<commit_message>
Changed x-axis from 'Cores' to 'Tasks' as suggested
Former-commit-id: 0637c074d45ef690e37acb9915da7aa3e7a1c4a5
</commit_message>
<xml_diff>
--- a/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
+++ b/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TTC_AIMES_SWIFT_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,19 +78,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF595959"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -272,7 +265,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -397,7 +390,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -497,11 +490,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78035479"/>
-        <c:axId val="88474536"/>
+        <c:axId val="82650270"/>
+        <c:axId val="20914808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78035479"/>
+        <c:axId val="82650270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +516,7 @@
                     </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Cores</a:t>
+                  <a:t>Tasks</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -541,14 +534,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88474536"/>
+        <c:crossAx val="20914808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88474536"/>
+        <c:axId val="20914808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25000"/>
@@ -596,7 +589,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="78035479"/>
+        <c:crossAx val="82650270"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -637,15 +630,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>693720</xdr:colOff>
+      <xdr:colOff>720720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>112320</xdr:colOff>
+      <xdr:colOff>138960</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -653,8 +646,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="693720" y="357480"/>
-        <a:ext cx="8400960" cy="4652640"/>
+        <a:off x="720720" y="348480"/>
+        <a:ext cx="8400600" cy="4652280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -826,10 +819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -964,6 +957,9 @@
         <v>15366.9908431</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -982,8 +978,8 @@
   </sheetPr>
   <dimension ref="A3:A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M42" activeCellId="0" sqref="M42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1000,6 +996,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Redoing the graphs, draft
</commit_message>
<xml_diff>
--- a/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
+++ b/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Timings_AIMES" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Plots" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Plot Data" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="33">
   <si>
     <t>TTC_AIMES_SWIFT_1_v2</t>
   </si>
@@ -81,10 +82,40 @@
     <t>Th_AIMES_SWIFT_3_v2</t>
   </si>
   <si>
+    <t>1 Resources</t>
+  </si>
+  <si>
     <t>Ts_AIMES_SWIFT_3_v2</t>
   </si>
   <si>
     <t>**BOLD Entries are NOT REAL. They are placeholder values to make the line plot continuous</t>
+  </si>
+  <si>
+    <t>TTC</t>
+  </si>
+  <si>
+    <t>2 Resource</t>
+  </si>
+  <si>
+    <t>IDEAL</t>
+  </si>
+  <si>
+    <t>Avg TTC</t>
+  </si>
+  <si>
+    <t>TTC_StDev</t>
+  </si>
+  <si>
+    <t>TTC_IDEAL</t>
+  </si>
+  <si>
+    <t>Tw</t>
+  </si>
+  <si>
+    <t>Avg Tw</t>
+  </si>
+  <si>
+    <t>Tw_StDev</t>
   </si>
 </sst>
 </file>
@@ -94,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,12 +155,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="13.2"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -273,7 +311,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1320">
+              <a:rPr b="1" sz="1320">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -316,7 +354,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -411,7 +449,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -506,7 +544,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -576,11 +614,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="22666360"/>
-        <c:axId val="56134935"/>
+        <c:axId val="99104006"/>
+        <c:axId val="55572140"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22666360"/>
+        <c:axId val="99104006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,7 +634,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -620,14 +658,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56134935"/>
+        <c:crossAx val="55572140"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56134935"/>
+        <c:axId val="55572140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +691,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -674,7 +712,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22666360"/>
+        <c:crossAx val="99104006"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -724,7 +762,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1320">
+              <a:rPr b="1" sz="1320">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -767,7 +805,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -776,38 +814,31 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
-            <c:noEndCap val="0"/>
-            <c:val val="0"/>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1020</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2050</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -869,7 +900,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -878,38 +909,31 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
-            <c:noEndCap val="0"/>
-            <c:val val="0"/>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1020</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2050</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -971,7 +995,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -980,38 +1004,31 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
-            <c:noEndCap val="0"/>
-            <c:val val="0"/>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1020</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2050</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1048,11 +1065,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="40087622"/>
-        <c:axId val="278167"/>
+        <c:axId val="28058145"/>
+        <c:axId val="4500132"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40087622"/>
+        <c:axId val="28058145"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1085,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1092,14 +1109,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="278167"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="4500132"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278167"/>
+        <c:axId val="4500132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000"/>
@@ -1126,7 +1143,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1147,7 +1164,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40087622"/>
+        <c:crossAx val="28058145"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1197,7 +1214,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1320">
+              <a:rPr b="1" sz="1320">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1240,7 +1257,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1249,72 +1266,6 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>1</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>21.8631076138</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>193.7554649122</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>6383.3760185485</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>11.05783916</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>659.771726</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8357.001755</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>622.09687</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>2</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>21.8631076138</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>193.7554649122</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>6383.3760185485</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>11.05783916</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>659.771726</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8357.001755</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>622.09687</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
@@ -1376,11 +1327,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="14729840"/>
-        <c:axId val="74261806"/>
+        <c:axId val="48734000"/>
+        <c:axId val="88125842"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14729840"/>
+        <c:axId val="48734000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1347,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1420,14 +1371,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74261806"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="88125842"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74261806"/>
+        <c:axId val="88125842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000"/>
@@ -1455,7 +1406,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1476,7 +1427,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14729840"/>
+        <c:crossAx val="48734000"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1526,7 +1477,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1320">
+              <a:rPr b="1" sz="1320">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1569,7 +1520,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1578,72 +1529,6 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>3</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>389.9532155416</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2.1150456386</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1576.2977787151</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>387.6494432</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6229.630339</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>710.4061733</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>115.4941312</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>4</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>389.9532155416</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2.1150456386</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1576.2977787151</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>387.6494432</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6229.630339</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>710.4061733</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>115.4941312</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
@@ -1705,11 +1590,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58184192"/>
-        <c:axId val="59662650"/>
+        <c:axId val="79564729"/>
+        <c:axId val="81692023"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58184192"/>
+        <c:axId val="79564729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1610,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1749,14 +1634,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59662650"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="81692023"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59662650"/>
+        <c:axId val="81692023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000"/>
@@ -1784,7 +1669,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1805,7 +1690,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58184192"/>
+        <c:crossAx val="79564729"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1855,7 +1740,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1320">
+              <a:rPr b="1" sz="1320">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1898,7 +1783,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1907,72 +1792,6 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>21.3459437563</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.2551485366</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.2551485366</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>625.4121816</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>6</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
-                  <c:pt idx="0">
-                    <c:v>21.3459437563</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.2551485366</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.2551485366</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>20.68826194</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>625.4121816</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>categories</c:f>
@@ -2034,11 +1853,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="2056049"/>
-        <c:axId val="17728933"/>
+        <c:axId val="78339825"/>
+        <c:axId val="32500644"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2056049"/>
+        <c:axId val="78339825"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2054,7 +1873,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2078,14 +1897,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17728933"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="32500644"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17728933"/>
+        <c:axId val="32500644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000"/>
@@ -2113,7 +1932,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1100">
+                  <a:rPr b="1" sz="1100">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2134,7 +1953,878 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2056049"/>
+        <c:crossAx val="78339825"/>
+        <c:crossesAt val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1320">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Tw - AIMES_Only</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tw_Resource_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="2"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>117.7780877</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259.4150921685</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.4687590605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9753.98555481</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tw_Resource_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="2"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>129.4008566</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118.0718771795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130.5777589673</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187.78897744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tw_Resource_4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92d050"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="92d050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="2"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>134.391339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.683530095</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140.19159406</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>209.619909075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="2847489"/>
+        <c:axId val="79773236"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2847489"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="79773236"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79773236"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2847489"/>
+        <c:crossesAt val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1320">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>TTC - AIMES_Only</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TTC_Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="333333"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="333333"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TTC_Resource_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1019.2150266765</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1162.7750162465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1022.47398907</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10703.97628748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TTC_Resource_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1708.1714770175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1034.898582695</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1591.784653245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3774.58370894</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TTC_Resource_4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92d050"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="92d050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1939.5044540175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1922.332989575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1971.5520235875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2835.0577372325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="6654810"/>
+        <c:axId val="54761201"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="6654810"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="54761201"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54761201"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1100">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="6654810"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2175,15 +2865,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>294120</xdr:colOff>
+      <xdr:colOff>348120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>265320</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>318600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2191,8 +2881,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9276480" y="315000"/>
-        <a:ext cx="8882280" cy="4718880"/>
+        <a:off x="9330480" y="297000"/>
+        <a:ext cx="8881560" cy="4718160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2205,15 +2895,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>741240</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>-360</xdr:rowOff>
+      <xdr:colOff>795240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>712800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:colOff>766080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2221,8 +2911,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="741240" y="324000"/>
-        <a:ext cx="8137440" cy="4719240"/>
+        <a:off x="795240" y="306000"/>
+        <a:ext cx="8136720" cy="4718520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2235,15 +2925,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>-360</xdr:colOff>
+      <xdr:colOff>53640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>787680</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>102600</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2251,8 +2941,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="816120" y="5279400"/>
-        <a:ext cx="8137440" cy="4719600"/>
+        <a:off x="870120" y="5261400"/>
+        <a:ext cx="8136720" cy="4718880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2265,15 +2955,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>323640</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>366480</xdr:colOff>
+      <xdr:colOff>419760</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2281,8 +2971,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9306000" y="5298120"/>
-        <a:ext cx="8137440" cy="4719600"/>
+        <a:off x="9360000" y="5280120"/>
+        <a:ext cx="8136720" cy="4718880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2295,15 +2985,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
+      <xdr:colOff>741960</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>659520</xdr:colOff>
+      <xdr:colOff>712800</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2311,12 +3001,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17764920" y="5326920"/>
-        <a:ext cx="8137440" cy="4719600"/>
+        <a:off x="17818920" y="5308920"/>
+        <a:ext cx="8136720" cy="4718880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>775080</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>81720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>745920</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="775080" y="15348240"/>
+        <a:ext cx="8136720" cy="4718520"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>794520</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>103320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>765360</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>107640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="794520" y="10492920"/>
+        <a:ext cx="8136720" cy="4718520"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2330,10 +3080,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI56"/>
+  <dimension ref="A1:AR41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2361,9 +3111,15 @@
         <v>1</v>
       </c>
       <c r="AB1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AM1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2464,6 +3220,30 @@
       <c r="AI3" s="0" t="n">
         <v>2048</v>
       </c>
+      <c r="AK3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>2048</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -2533,61 +3313,92 @@
       </c>
       <c r="T5" s="0" t="n">
         <f aca="false">AVERAGE(T8:T11)</f>
-        <v>20.054939568025</v>
+        <v>134.391339005</v>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">AVERAGE(U8:U11)</f>
-        <v>21.1941587925</v>
-      </c>
-      <c r="V5" s="1" t="n">
+        <v>117.683530095</v>
+      </c>
+      <c r="V5" s="0" t="n">
         <f aca="false">AVERAGE(V8:V11)</f>
-        <v>21.1941587925</v>
+        <v>118.683530095</v>
       </c>
       <c r="W5" s="0" t="n">
         <f aca="false">AVERAGE(W8:W11)</f>
-        <v>26.0237275362</v>
-      </c>
-      <c r="X5" s="1" t="n">
+        <v>140.19159406</v>
+      </c>
+      <c r="X5" s="0" t="n">
         <f aca="false">AVERAGE(X8:X11)</f>
-        <v>26.0237275362</v>
-      </c>
-      <c r="Y5" s="1" t="n">
+        <v>141.19159406</v>
+      </c>
+      <c r="Y5" s="0" t="n">
         <f aca="false">AVERAGE(Y8:Y11)</f>
-        <v>26.0237275362</v>
+        <v>142.19159406</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">AVERAGE(Z8:Z11)</f>
-        <v>101.9300326704</v>
+        <v>209.6199097075</v>
       </c>
       <c r="AB5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">AVERAGE(AC8:AC11)</f>
-        <v>20.8808839321225</v>
+        <v>20.054939568025</v>
       </c>
       <c r="AD5" s="0" t="n">
         <f aca="false">AVERAGE(AD8:AD11)</f>
-        <v>18.30193263293</v>
-      </c>
-      <c r="AE5" s="0" t="n">
+        <v>21.1941587925</v>
+      </c>
+      <c r="AE5" s="1" t="n">
         <f aca="false">AVERAGE(AE8:AE11)</f>
-        <v>18.30193263293</v>
+        <v>21.1941587925</v>
       </c>
       <c r="AF5" s="0" t="n">
         <f aca="false">AVERAGE(AF8:AF11)</f>
-        <v>58.609807312475</v>
-      </c>
-      <c r="AG5" s="0" t="n">
+        <v>26.0237275362</v>
+      </c>
+      <c r="AG5" s="1" t="n">
         <f aca="false">AVERAGE(AG8:AG11)</f>
-        <v>58.609807312475</v>
-      </c>
-      <c r="AH5" s="0" t="n">
+        <v>26.0237275362</v>
+      </c>
+      <c r="AH5" s="1" t="n">
         <f aca="false">AVERAGE(AH8:AH11)</f>
-        <v>58.609807312475</v>
+        <v>26.0237275362</v>
       </c>
       <c r="AI5" s="0" t="n">
         <f aca="false">AVERAGE(AI8:AI11)</f>
+        <v>101.9300326704</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <f aca="false">AVERAGE(AL8:AL11)</f>
+        <v>20.8808839321225</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <f aca="false">AVERAGE(AM8:AM11)</f>
+        <v>18.30193263293</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <f aca="false">AVERAGE(AN8:AN11)</f>
+        <v>18.30193263293</v>
+      </c>
+      <c r="AO5" s="0" t="n">
+        <f aca="false">AVERAGE(AO8:AO11)</f>
+        <v>58.609807312475</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <f aca="false">AVERAGE(AP8:AP11)</f>
+        <v>58.609807312475</v>
+      </c>
+      <c r="AQ5" s="0" t="n">
+        <f aca="false">AVERAGE(AQ8:AQ11)</f>
+        <v>58.609807312475</v>
+      </c>
+      <c r="AR5" s="0" t="n">
+        <f aca="false">AVERAGE(AR8:AR11)</f>
         <v>1166.66731926925</v>
       </c>
     </row>
@@ -2659,61 +3470,92 @@
       </c>
       <c r="T6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(T8:T11)</f>
-        <v>2.69060420429174</v>
+        <v>22.0923253591981</v>
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(U8:U11)</f>
-        <v>5.70035704079912</v>
-      </c>
-      <c r="V6" s="1" t="n">
+        <v>4.82326564498172</v>
+      </c>
+      <c r="V6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(V8:V11)</f>
-        <v>5.70035704079912</v>
+        <v>4.82326564498172</v>
       </c>
       <c r="W6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(W8:W11)</f>
-        <v>3.88801433736543</v>
-      </c>
-      <c r="X6" s="1" t="n">
+        <v>6.23869432135785</v>
+      </c>
+      <c r="X6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(X8:X11)</f>
-        <v>3.88801433736543</v>
-      </c>
-      <c r="Y6" s="1" t="n">
+        <v>6.23869432135785</v>
+      </c>
+      <c r="Y6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Y8:Y11)</f>
-        <v>3.88801433736543</v>
+        <v>6.23869432135785</v>
       </c>
       <c r="Z6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Z8:Z11)</f>
-        <v>9.00271558019951</v>
+        <v>5.41536815417673</v>
       </c>
       <c r="AB6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="AC6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AC8:AC11)</f>
-        <v>1.5317051420217</v>
+        <v>2.69060420429174</v>
       </c>
       <c r="AD6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AD8:AD11)</f>
-        <v>6.45355516141529</v>
-      </c>
-      <c r="AE6" s="0" t="n">
+        <v>5.70035704079912</v>
+      </c>
+      <c r="AE6" s="1" t="n">
         <f aca="false">_xlfn.STDEV.P(AE8:AE11)</f>
-        <v>6.45355516141529</v>
+        <v>5.70035704079912</v>
       </c>
       <c r="AF6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AF8:AF11)</f>
-        <v>20.3589309780087</v>
-      </c>
-      <c r="AG6" s="0" t="n">
+        <v>3.88801433736543</v>
+      </c>
+      <c r="AG6" s="1" t="n">
         <f aca="false">_xlfn.STDEV.P(AG8:AG11)</f>
-        <v>20.3589309780087</v>
-      </c>
-      <c r="AH6" s="0" t="n">
+        <v>3.88801433736543</v>
+      </c>
+      <c r="AH6" s="1" t="n">
         <f aca="false">_xlfn.STDEV.P(AH8:AH11)</f>
-        <v>20.3589309780087</v>
+        <v>3.88801433736543</v>
       </c>
       <c r="AI6" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AI8:AI11)</f>
+        <v>9.00271558019951</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AL8:AL11)</f>
+        <v>1.5317051420217</v>
+      </c>
+      <c r="AM6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AM8:AM11)</f>
+        <v>6.45355516141529</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AN8:AN11)</f>
+        <v>6.45355516141529</v>
+      </c>
+      <c r="AO6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AO8:AO11)</f>
+        <v>20.3589309780087</v>
+      </c>
+      <c r="AP6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AP8:AP11)</f>
+        <v>20.3589309780087</v>
+      </c>
+      <c r="AQ6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AQ8:AQ11)</f>
+        <v>20.3589309780087</v>
+      </c>
+      <c r="AR6" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AR8:AR11)</f>
         <v>705.496400135275</v>
       </c>
     </row>
@@ -2724,9 +3566,9 @@
       <c r="M7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -2781,48 +3623,79 @@
         <v>8</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>20.9471969604</v>
+        <f aca="false">B8-K8</f>
+        <v>126.00367785</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>28.7104930878</v>
-      </c>
-      <c r="V8" s="1" t="n">
-        <v>28.7104930878</v>
+        <f aca="false">C8-L8</f>
+        <v>113.59935403</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <f aca="false">D8-M8</f>
+        <v>114.59935403</v>
       </c>
       <c r="W8" s="0" t="n">
-        <v>26.0957019329</v>
-      </c>
-      <c r="X8" s="1" t="n">
-        <v>26.0957019329</v>
-      </c>
-      <c r="Y8" s="1" t="n">
-        <v>26.0957019329</v>
+        <f aca="false">E8-N8</f>
+        <v>150.74305105</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <f aca="false">F8-O8</f>
+        <v>151.74305105</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <f aca="false">G8-P8</f>
+        <v>152.74305105</v>
       </c>
       <c r="Z8" s="0" t="n">
-        <v>102.020359039</v>
+        <f aca="false">H8-Q8</f>
+        <v>208.54335213</v>
       </c>
       <c r="AB8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="AC8" s="0" t="n">
+        <v>20.9471969604</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <v>28.7104930878</v>
+      </c>
+      <c r="AE8" s="1" t="n">
+        <v>28.7104930878</v>
+      </c>
+      <c r="AF8" s="0" t="n">
+        <v>26.0957019329</v>
+      </c>
+      <c r="AG8" s="1" t="n">
+        <v>26.0957019329</v>
+      </c>
+      <c r="AH8" s="1" t="n">
+        <v>26.0957019329</v>
+      </c>
+      <c r="AI8" s="0" t="n">
+        <v>102.020359039</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL8" s="0" t="n">
         <v>20.63821291922</v>
       </c>
-      <c r="AD8" s="0" t="n">
+      <c r="AM8" s="0" t="n">
         <v>9.70534992218</v>
       </c>
-      <c r="AE8" s="0" t="n">
+      <c r="AN8" s="0" t="n">
         <v>9.70534992218</v>
       </c>
-      <c r="AF8" s="0" t="n">
+      <c r="AO8" s="0" t="n">
         <v>84.4051742553</v>
       </c>
-      <c r="AG8" s="0" t="n">
+      <c r="AP8" s="0" t="n">
         <v>84.4051742553</v>
       </c>
-      <c r="AH8" s="0" t="n">
+      <c r="AQ8" s="0" t="n">
         <v>84.4051742553</v>
       </c>
-      <c r="AI8" s="0" t="n">
+      <c r="AR8" s="0" t="n">
         <v>795.761815667</v>
       </c>
     </row>
@@ -2879,48 +3752,79 @@
         <v>9</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>20.7203850746</v>
+        <f aca="false">B9-K9</f>
+        <v>170.7058928</v>
       </c>
       <c r="U9" s="0" t="n">
-        <v>24.4420330524</v>
-      </c>
-      <c r="V9" s="1" t="n">
-        <v>24.4420330524</v>
+        <f aca="false">C9-L9</f>
+        <v>113.057899</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <f aca="false">D9-M9</f>
+        <v>114.057899</v>
       </c>
       <c r="W9" s="0" t="n">
-        <v>19.6510469913</v>
-      </c>
-      <c r="X9" s="1" t="n">
-        <v>19.6510469913</v>
-      </c>
-      <c r="Y9" s="1" t="n">
-        <v>19.6510469913</v>
+        <f aca="false">E9-N9</f>
+        <v>136.32205438</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <f aca="false">F9-O9</f>
+        <v>137.32205438</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <f aca="false">G9-P9</f>
+        <v>138.32205438</v>
       </c>
       <c r="Z9" s="0" t="n">
-        <v>110.035069942</v>
+        <f aca="false">H9-Q9</f>
+        <v>218.66549397</v>
       </c>
       <c r="AB9" s="0" t="s">
         <v>9</v>
       </c>
       <c r="AC9" s="0" t="n">
+        <v>20.7203850746</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>24.4420330524</v>
+      </c>
+      <c r="AE9" s="1" t="n">
+        <v>24.4420330524</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>19.6510469913</v>
+      </c>
+      <c r="AG9" s="1" t="n">
+        <v>19.6510469913</v>
+      </c>
+      <c r="AH9" s="1" t="n">
+        <v>19.6510469913</v>
+      </c>
+      <c r="AI9" s="0" t="n">
+        <v>110.035069942</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL9" s="0" t="n">
         <v>18.60934829716</v>
       </c>
-      <c r="AD9" s="0" t="n">
+      <c r="AM9" s="0" t="n">
         <v>14.64428687096</v>
       </c>
-      <c r="AE9" s="0" t="n">
+      <c r="AN9" s="0" t="n">
         <v>14.64428687096</v>
       </c>
-      <c r="AF9" s="0" t="n">
+      <c r="AO9" s="0" t="n">
         <v>48.2130622864</v>
       </c>
-      <c r="AG9" s="0" t="n">
+      <c r="AP9" s="0" t="n">
         <v>48.2130622864</v>
       </c>
-      <c r="AH9" s="0" t="n">
+      <c r="AQ9" s="0" t="n">
         <v>48.2130622864</v>
       </c>
-      <c r="AI9" s="0" t="n">
+      <c r="AR9" s="0" t="n">
         <v>750.457919121</v>
       </c>
     </row>
@@ -2977,48 +3881,79 @@
         <v>10</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>22.916503191</v>
+        <f aca="false">B10-K10</f>
+        <v>129.73455739</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>17.392911911</v>
-      </c>
-      <c r="V10" s="1" t="n">
-        <v>17.392911911</v>
+        <f aca="false">C10-L10</f>
+        <v>119.11882425</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <f aca="false">D10-M10</f>
+        <v>120.11882425</v>
       </c>
       <c r="W10" s="0" t="n">
-        <v>29.1524550915</v>
-      </c>
-      <c r="X10" s="1" t="n">
-        <v>29.1524550915</v>
-      </c>
-      <c r="Y10" s="1" t="n">
-        <v>29.1524550915</v>
+        <f aca="false">E10-N10</f>
+        <v>138.72875094</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <f aca="false">F10-O10</f>
+        <v>139.72875094</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <f aca="false">G10-P10</f>
+        <v>140.72875094</v>
       </c>
       <c r="Z10" s="0" t="n">
-        <v>87.2277817726</v>
+        <f aca="false">H10-Q10</f>
+        <v>206.76910377</v>
       </c>
       <c r="AB10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="AC10" s="0" t="n">
+        <v>22.916503191</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>17.392911911</v>
+      </c>
+      <c r="AE10" s="1" t="n">
+        <v>17.392911911</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>29.1524550915</v>
+      </c>
+      <c r="AG10" s="1" t="n">
+        <v>29.1524550915</v>
+      </c>
+      <c r="AH10" s="1" t="n">
+        <v>29.1524550915</v>
+      </c>
+      <c r="AI10" s="0" t="n">
+        <v>87.2277817726</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL10" s="0" t="n">
         <v>21.42907905576</v>
       </c>
-      <c r="AD10" s="0" t="n">
+      <c r="AM10" s="0" t="n">
         <v>22.97459983827</v>
       </c>
-      <c r="AE10" s="0" t="n">
+      <c r="AN10" s="0" t="n">
         <v>22.97459983827</v>
       </c>
-      <c r="AF10" s="0" t="n">
+      <c r="AO10" s="0" t="n">
         <v>31.3414871693</v>
       </c>
-      <c r="AG10" s="0" t="n">
+      <c r="AP10" s="0" t="n">
         <v>31.3414871693</v>
       </c>
-      <c r="AH10" s="0" t="n">
+      <c r="AQ10" s="0" t="n">
         <v>31.3414871693</v>
       </c>
-      <c r="AI10" s="0" t="n">
+      <c r="AR10" s="0" t="n">
         <v>2387.97007895</v>
       </c>
     </row>
@@ -3075,48 +4010,79 @@
         <v>11</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>15.6356730461</v>
+        <f aca="false">B11-K11</f>
+        <v>111.12122798</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>14.2311971188</v>
-      </c>
-      <c r="V11" s="1" t="n">
-        <v>14.2311971188</v>
+        <f aca="false">C11-L11</f>
+        <v>124.9580431</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <f aca="false">D11-M11</f>
+        <v>125.9580431</v>
       </c>
       <c r="W11" s="0" t="n">
-        <v>29.1957061291</v>
-      </c>
-      <c r="X11" s="1" t="n">
-        <v>29.1957061291</v>
-      </c>
-      <c r="Y11" s="1" t="n">
-        <v>29.1957061291</v>
+        <f aca="false">E11-N11</f>
+        <v>134.97251987</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <f aca="false">F11-O11</f>
+        <v>135.97251987</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <f aca="false">G11-P11</f>
+        <v>136.97251987</v>
       </c>
       <c r="Z11" s="0" t="n">
-        <v>108.436919928</v>
+        <f aca="false">H11-Q11</f>
+        <v>204.50168896</v>
       </c>
       <c r="AB11" s="0" t="s">
         <v>11</v>
       </c>
       <c r="AC11" s="0" t="n">
+        <v>15.6356730461</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <v>14.2311971188</v>
+      </c>
+      <c r="AE11" s="1" t="n">
+        <v>14.2311971188</v>
+      </c>
+      <c r="AF11" s="0" t="n">
+        <v>29.1957061291</v>
+      </c>
+      <c r="AG11" s="1" t="n">
+        <v>29.1957061291</v>
+      </c>
+      <c r="AH11" s="1" t="n">
+        <v>29.1957061291</v>
+      </c>
+      <c r="AI11" s="0" t="n">
+        <v>108.436919928</v>
+      </c>
+      <c r="AK11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL11" s="0" t="n">
         <v>22.84689545635</v>
       </c>
-      <c r="AD11" s="0" t="n">
+      <c r="AM11" s="0" t="n">
         <v>25.88349390031</v>
       </c>
-      <c r="AE11" s="0" t="n">
+      <c r="AN11" s="0" t="n">
         <v>25.88349390031</v>
       </c>
-      <c r="AF11" s="0" t="n">
+      <c r="AO11" s="0" t="n">
         <v>70.4795055389</v>
       </c>
-      <c r="AG11" s="0" t="n">
+      <c r="AP11" s="0" t="n">
         <v>70.4795055389</v>
       </c>
-      <c r="AH11" s="0" t="n">
+      <c r="AQ11" s="0" t="n">
         <v>70.4795055389</v>
       </c>
-      <c r="AI11" s="0" t="n">
+      <c r="AR11" s="0" t="n">
         <v>732.479463339</v>
       </c>
     </row>
@@ -3140,6 +4106,12 @@
         <v>13</v>
       </c>
       <c r="AB14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK14" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3240,6 +4212,30 @@
       <c r="AI16" s="0" t="n">
         <v>2048</v>
       </c>
+      <c r="AK16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM16" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AN16" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="AO16" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="AP16" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="AQ16" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="AR16" s="0" t="n">
+        <v>2048</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -3309,49 +4305,80 @@
       </c>
       <c r="T18" s="0" t="n">
         <f aca="false">AVERAGE(T21:T24)</f>
-        <v>12.9212062954925</v>
+        <v>129.40085655175</v>
       </c>
       <c r="U18" s="0" t="n">
         <f aca="false">AVERAGE(U21:U24)</f>
-        <v>17.89685952665</v>
+        <v>118.0718771795</v>
       </c>
       <c r="V18" s="0" t="n">
         <f aca="false">AVERAGE(V21:V24)</f>
-        <v>2179.287987708</v>
+        <v>2284.49642646</v>
       </c>
       <c r="W18" s="0" t="n">
         <f aca="false">AVERAGE(W21:W24)</f>
-        <v>20.161033988025</v>
+        <v>130.57775896725</v>
       </c>
       <c r="X18" s="0" t="n">
         <f aca="false">AVERAGE(X21:X24)</f>
-        <v>7573.1237204575</v>
+        <v>7695.8659844275</v>
       </c>
       <c r="Y18" s="0" t="n">
         <f aca="false">AVERAGE(Y21:Y24)</f>
-        <v>1108.41065621425</v>
+        <v>1237.41018832</v>
       </c>
       <c r="Z18" s="0" t="n">
         <f aca="false">AVERAGE(Z21:Z24)</f>
-        <v>88.3177791834</v>
+        <v>184.78897744</v>
       </c>
       <c r="AB18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="AC18" s="0" t="n">
         <f aca="false">AVERAGE(AC21:AC24)</f>
-        <v>13.776561439015</v>
+        <v>12.9212062954925</v>
       </c>
       <c r="AD18" s="0" t="n">
         <f aca="false">AVERAGE(AD21:AD24)</f>
-        <v>21.1279565691975</v>
+        <v>17.89685952665</v>
+      </c>
+      <c r="AE18" s="0" t="n">
+        <f aca="false">AVERAGE(AE21:AE24)</f>
+        <v>2179.287987708</v>
       </c>
       <c r="AF18" s="0" t="n">
         <f aca="false">AVERAGE(AF21:AF24)</f>
-        <v>58.38007801775</v>
+        <v>20.161033988025</v>
+      </c>
+      <c r="AG18" s="0" t="n">
+        <f aca="false">AVERAGE(AG21:AG24)</f>
+        <v>7573.1237204575</v>
+      </c>
+      <c r="AH18" s="0" t="n">
+        <f aca="false">AVERAGE(AH21:AH24)</f>
+        <v>1108.41065621425</v>
       </c>
       <c r="AI18" s="0" t="n">
         <f aca="false">AVERAGE(AI21:AI24)</f>
+        <v>88.3177791834</v>
+      </c>
+      <c r="AK18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <f aca="false">AVERAGE(AL21:AL24)</f>
+        <v>13.776561439015</v>
+      </c>
+      <c r="AM18" s="0" t="n">
+        <f aca="false">AVERAGE(AM21:AM24)</f>
+        <v>21.1279565691975</v>
+      </c>
+      <c r="AO18" s="0" t="n">
+        <f aca="false">AVERAGE(AO21:AO24)</f>
+        <v>58.38007801775</v>
+      </c>
+      <c r="AR18" s="0" t="n">
+        <f aca="false">AVERAGE(AR21:AR24)</f>
         <v>2409.53850531775</v>
       </c>
     </row>
@@ -3423,49 +4450,80 @@
       </c>
       <c r="T19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(T21:T24)</f>
-        <v>2.37846760232575</v>
+        <v>8.30532410306872</v>
       </c>
       <c r="U19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(U21:U24)</f>
-        <v>6.85630263369234</v>
+        <v>11.0461881096775</v>
       </c>
       <c r="V19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(V21:V24)</f>
-        <v>1561.01727936946</v>
+        <v>1555.63880556449</v>
       </c>
       <c r="W19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(W21:W24)</f>
-        <v>3.62430366793779</v>
+        <v>9.84240349163049</v>
       </c>
       <c r="X19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(X21:X24)</f>
-        <v>6214.93628230041</v>
+        <v>6214.20896556445</v>
       </c>
       <c r="Y19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Y21:Y24)</f>
-        <v>789.832716786609</v>
+        <v>795.454197507782</v>
       </c>
       <c r="Z19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Z21:Z24)</f>
-        <v>4.02599594449866</v>
+        <v>18.2364689097185</v>
       </c>
       <c r="AB19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="AC19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AC21:AC24)</f>
-        <v>2.91914713364881</v>
+        <v>2.37846760232575</v>
       </c>
       <c r="AD19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AD21:AD24)</f>
-        <v>3.51962109238171</v>
+        <v>6.85630263369234</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AE21:AE24)</f>
+        <v>1561.01727936946</v>
       </c>
       <c r="AF19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AF21:AF24)</f>
-        <v>15.5009596864169</v>
+        <v>3.62430366793779</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AG21:AG24)</f>
+        <v>6214.93628230041</v>
+      </c>
+      <c r="AH19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AH21:AH24)</f>
+        <v>789.832716786609</v>
       </c>
       <c r="AI19" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AI21:AI24)</f>
+        <v>4.02599594449866</v>
+      </c>
+      <c r="AK19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AL21:AL24)</f>
+        <v>2.91914713364881</v>
+      </c>
+      <c r="AM19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AM21:AM24)</f>
+        <v>3.51962109238171</v>
+      </c>
+      <c r="AO19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AO21:AO24)</f>
+        <v>15.5009596864169</v>
+      </c>
+      <c r="AR19" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AR21:AR24)</f>
         <v>100.880589320032</v>
       </c>
     </row>
@@ -3522,39 +4580,70 @@
         <v>8</v>
       </c>
       <c r="T21" s="0" t="n">
-        <v>16.1224091053</v>
+        <f aca="false">B21-K21</f>
+        <v>119.84542823</v>
       </c>
       <c r="U21" s="0" t="n">
-        <v>11.4463131428</v>
+        <f aca="false">C21-L21</f>
+        <v>103.112755778</v>
       </c>
       <c r="V21" s="0" t="n">
-        <v>1157.0327239</v>
+        <f aca="false">D21-M21</f>
+        <v>1281.3277769</v>
       </c>
       <c r="W21" s="0" t="n">
-        <v>25.2811610699</v>
+        <f aca="false">E21-N21</f>
+        <v>122.231108189</v>
       </c>
       <c r="X21" s="0" t="n">
-        <v>7048.78994894</v>
+        <f aca="false">F21-O21</f>
+        <v>7185.06898236</v>
       </c>
       <c r="Y21" s="0" t="n">
-        <v>2081.52934694</v>
+        <f aca="false">G21-P21</f>
+        <v>2206.50690413</v>
       </c>
       <c r="Z21" s="0" t="n">
-        <v>88.147687912</v>
+        <f aca="false">H21-Q21</f>
+        <v>160.42066788</v>
       </c>
       <c r="AB21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="AC21" s="0" t="n">
+        <v>16.1224091053</v>
+      </c>
+      <c r="AD21" s="0" t="n">
+        <v>11.4463131428</v>
+      </c>
+      <c r="AE21" s="0" t="n">
+        <v>1157.0327239</v>
+      </c>
+      <c r="AF21" s="0" t="n">
+        <v>25.2811610699</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <v>7048.78994894</v>
+      </c>
+      <c r="AH21" s="0" t="n">
+        <v>2081.52934694</v>
+      </c>
+      <c r="AI21" s="0" t="n">
+        <v>88.147687912</v>
+      </c>
+      <c r="AK21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL21" s="0" t="n">
         <v>9.04602098465</v>
       </c>
-      <c r="AD21" s="0" t="n">
+      <c r="AM21" s="0" t="n">
         <v>22.56521010403</v>
       </c>
-      <c r="AF21" s="0" t="n">
+      <c r="AO21" s="0" t="n">
         <v>35.5087213517</v>
       </c>
-      <c r="AI21" s="0" t="n">
+      <c r="AR21" s="0" t="n">
         <v>2254.019945505</v>
       </c>
     </row>
@@ -3611,39 +4700,70 @@
         <v>9</v>
       </c>
       <c r="T22" s="0" t="n">
-        <v>9.48660111427</v>
+        <f aca="false">B22-K22</f>
+        <v>135.50799894</v>
       </c>
       <c r="U22" s="0" t="n">
-        <v>15.818073988</v>
+        <f aca="false">C22-L22</f>
+        <v>133.668916937</v>
       </c>
       <c r="V22" s="0" t="n">
-        <v>716.895250082</v>
+        <f aca="false">D22-M22</f>
+        <v>807.45179511</v>
       </c>
       <c r="W22" s="0" t="n">
-        <v>19.6727318764</v>
+        <f aca="false">E22-N22</f>
+        <v>143.33517885</v>
       </c>
       <c r="X22" s="0" t="n">
-        <v>825.41800499</v>
+        <f aca="false">F22-O22</f>
+        <v>948.49650216</v>
       </c>
       <c r="Y22" s="0" t="n">
-        <v>63.072893858</v>
+        <f aca="false">G22-P22</f>
+        <v>193.90969825</v>
       </c>
       <c r="Z22" s="0" t="n">
-        <v>81.8684148788</v>
+        <f aca="false">H22-Q22</f>
+        <v>176.32802319</v>
       </c>
       <c r="AB22" s="0" t="s">
         <v>9</v>
       </c>
       <c r="AC22" s="0" t="n">
+        <v>9.48660111427</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>15.818073988</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <v>716.895250082</v>
+      </c>
+      <c r="AF22" s="0" t="n">
+        <v>19.6727318764</v>
+      </c>
+      <c r="AG22" s="0" t="n">
+        <v>825.41800499</v>
+      </c>
+      <c r="AH22" s="0" t="n">
+        <v>63.072893858</v>
+      </c>
+      <c r="AI22" s="0" t="n">
+        <v>81.8684148788</v>
+      </c>
+      <c r="AK22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL22" s="0" t="n">
         <v>16.02340412137</v>
       </c>
-      <c r="AD22" s="0" t="n">
+      <c r="AM22" s="0" t="n">
         <v>17.21511006352</v>
       </c>
-      <c r="AF22" s="0" t="n">
+      <c r="AO22" s="0" t="n">
         <v>54.5140800476</v>
       </c>
-      <c r="AI22" s="0" t="n">
+      <c r="AR22" s="0" t="n">
         <v>2529.09274042</v>
       </c>
     </row>
@@ -3700,39 +4820,70 @@
         <v>10</v>
       </c>
       <c r="T23" s="0" t="n">
-        <v>13.5656299591</v>
+        <f aca="false">B23-K23</f>
+        <v>122.717714067</v>
       </c>
       <c r="U23" s="0" t="n">
-        <v>14.8906970024</v>
+        <f aca="false">C23-L23</f>
+        <v>114.525949238</v>
       </c>
       <c r="V23" s="0" t="n">
-        <v>2103.13491297</v>
+        <f aca="false">D23-M23</f>
+        <v>2217.63879203</v>
       </c>
       <c r="W23" s="0" t="n">
-        <v>15.0737259388</v>
+        <f aca="false">E23-N23</f>
+        <v>136.89721584</v>
       </c>
       <c r="X23" s="0" t="n">
-        <v>17622.1768529</v>
+        <f aca="false">F23-O23</f>
+        <v>17741.224369</v>
       </c>
       <c r="Y23" s="0" t="n">
-        <v>1620.46349812</v>
+        <f aca="false">G23-P23</f>
+        <v>1774.70198894</v>
       </c>
       <c r="Z23" s="0" t="n">
-        <v>90.8204300404</v>
+        <f aca="false">H23-Q23</f>
+        <v>209.14063191</v>
       </c>
       <c r="AB23" s="0" t="s">
         <v>10</v>
       </c>
       <c r="AC23" s="0" t="n">
+        <v>13.5656299591</v>
+      </c>
+      <c r="AD23" s="0" t="n">
+        <v>14.8906970024</v>
+      </c>
+      <c r="AE23" s="0" t="n">
+        <v>2103.13491297</v>
+      </c>
+      <c r="AF23" s="0" t="n">
+        <v>15.0737259388</v>
+      </c>
+      <c r="AG23" s="0" t="n">
+        <v>17622.1768529</v>
+      </c>
+      <c r="AH23" s="0" t="n">
+        <v>1620.46349812</v>
+      </c>
+      <c r="AI23" s="0" t="n">
+        <v>90.8204300404</v>
+      </c>
+      <c r="AK23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL23" s="0" t="n">
         <v>16.35538220404</v>
       </c>
-      <c r="AD23" s="0" t="n">
+      <c r="AM23" s="0" t="n">
         <v>26.18089294437</v>
       </c>
-      <c r="AF23" s="0" t="n">
+      <c r="AO23" s="0" t="n">
         <v>77.4772386551</v>
       </c>
-      <c r="AI23" s="0" t="n">
+      <c r="AR23" s="0" t="n">
         <v>2399.399329661</v>
       </c>
     </row>
@@ -3789,39 +4940,70 @@
         <v>11</v>
       </c>
       <c r="T24" s="0" t="n">
-        <v>12.5101850033</v>
+        <f aca="false">B24-K24</f>
+        <v>139.53228497</v>
       </c>
       <c r="U24" s="0" t="n">
-        <v>29.4323539734</v>
+        <f aca="false">C24-L24</f>
+        <v>120.979886765</v>
       </c>
       <c r="V24" s="0" t="n">
-        <v>4740.08906388</v>
+        <f aca="false">D24-M24</f>
+        <v>4831.5673418</v>
       </c>
       <c r="W24" s="0" t="n">
-        <v>20.616517067</v>
+        <f aca="false">E24-N24</f>
+        <v>119.84753299</v>
       </c>
       <c r="X24" s="0" t="n">
-        <v>4796.110075</v>
+        <f aca="false">F24-O24</f>
+        <v>4908.67408419</v>
       </c>
       <c r="Y24" s="0" t="n">
-        <v>668.576885939</v>
+        <f aca="false">G24-P24</f>
+        <v>774.52216196</v>
       </c>
       <c r="Z24" s="0" t="n">
-        <v>92.4345839024</v>
+        <f aca="false">H24-Q24</f>
+        <v>193.26658678</v>
       </c>
       <c r="AB24" s="0" t="s">
         <v>11</v>
       </c>
       <c r="AC24" s="0" t="n">
+        <v>12.5101850033</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <v>29.4323539734</v>
+      </c>
+      <c r="AE24" s="0" t="n">
+        <v>4740.08906388</v>
+      </c>
+      <c r="AF24" s="0" t="n">
+        <v>20.616517067</v>
+      </c>
+      <c r="AG24" s="0" t="n">
+        <v>4796.110075</v>
+      </c>
+      <c r="AH24" s="0" t="n">
+        <v>668.576885939</v>
+      </c>
+      <c r="AI24" s="0" t="n">
+        <v>92.4345839024</v>
+      </c>
+      <c r="AK24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL24" s="0" t="n">
         <v>13.681438446</v>
       </c>
-      <c r="AD24" s="0" t="n">
+      <c r="AM24" s="0" t="n">
         <v>18.55061316487</v>
       </c>
-      <c r="AF24" s="0" t="n">
+      <c r="AO24" s="0" t="n">
         <v>66.0202720166</v>
       </c>
-      <c r="AI24" s="0" t="n">
+      <c r="AR24" s="0" t="n">
         <v>2455.642005685</v>
       </c>
     </row>
@@ -3842,10 +5024,16 @@
         <v>20</v>
       </c>
       <c r="U27" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD27" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="AB27" s="0" t="s">
-        <v>21</v>
+      <c r="AK27" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,6 +5133,30 @@
       <c r="AI29" s="0" t="n">
         <v>2048</v>
       </c>
+      <c r="AK29" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL29" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM29" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AN29" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="AO29" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="AP29" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="AQ29" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="AR29" s="0" t="n">
+        <v>2048</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -4014,61 +5226,92 @@
       </c>
       <c r="T31" s="0" t="n">
         <f aca="false">AVERAGE(T34:T37)</f>
-        <v>5.8833917379375</v>
+        <v>117.77808773525</v>
       </c>
       <c r="U31" s="0" t="n">
         <f aca="false">AVERAGE(U34:U37)</f>
-        <v>7.42077231407</v>
+        <v>259.4150921685</v>
       </c>
       <c r="V31" s="0" t="n">
         <f aca="false">AVERAGE(V34:V37)</f>
-        <v>6053.67346226145</v>
+        <v>6126.57372480025</v>
       </c>
       <c r="W31" s="0" t="n">
         <f aca="false">AVERAGE(W34:W37)</f>
-        <v>11.206987023365</v>
+        <v>111.4687590605</v>
       </c>
       <c r="X31" s="0" t="n">
         <f aca="false">AVERAGE(X34:X37)</f>
-        <v>792.187748074675</v>
+        <v>870.64085799275</v>
       </c>
       <c r="Y31" s="0" t="n">
         <f aca="false">AVERAGE(Y34:Y37)</f>
-        <v>12006.1372189643</v>
+        <v>16728.1907179833</v>
       </c>
       <c r="Z31" s="0" t="n">
         <f aca="false">AVERAGE(Z34:Z37)</f>
-        <v>41.56971293685</v>
+        <v>9753.98555481</v>
       </c>
       <c r="AB31" s="0" t="s">
         <v>6</v>
       </c>
       <c r="AC31" s="0" t="n">
         <f aca="false">AVERAGE(AC34:AC37)</f>
-        <v>98.88782370102</v>
+        <v>5.8833917379375</v>
       </c>
       <c r="AD31" s="0" t="n">
         <f aca="false">AVERAGE(AD34:AD37)</f>
-        <v>240.380842983695</v>
+        <v>7.42077231407</v>
       </c>
       <c r="AE31" s="0" t="n">
         <f aca="false">AVERAGE(AE34:AE37)</f>
-        <v>39.427557170375</v>
+        <v>6053.67346226145</v>
       </c>
       <c r="AF31" s="0" t="n">
         <f aca="false">AVERAGE(AF34:AF37)</f>
-        <v>93.908548176225</v>
+        <v>11.206987023365</v>
       </c>
       <c r="AG31" s="0" t="n">
         <f aca="false">AVERAGE(AG34:AG37)</f>
-        <v>48.17433023455</v>
+        <v>792.187748074675</v>
       </c>
       <c r="AH31" s="0" t="n">
         <f aca="false">AVERAGE(AH34:AH37)</f>
-        <v>54.543495059</v>
+        <v>12006.1372189643</v>
       </c>
       <c r="AI31" s="0" t="n">
         <f aca="false">AVERAGE(AI34:AI37)</f>
+        <v>41.56971293685</v>
+      </c>
+      <c r="AK31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL31" s="0" t="n">
+        <f aca="false">AVERAGE(AL34:AL37)</f>
+        <v>98.88782370102</v>
+      </c>
+      <c r="AM31" s="0" t="n">
+        <f aca="false">AVERAGE(AM34:AM37)</f>
+        <v>240.380842983695</v>
+      </c>
+      <c r="AN31" s="0" t="n">
+        <f aca="false">AVERAGE(AN34:AN37)</f>
+        <v>39.427557170375</v>
+      </c>
+      <c r="AO31" s="0" t="n">
+        <f aca="false">AVERAGE(AO34:AO37)</f>
+        <v>93.908548176225</v>
+      </c>
+      <c r="AP31" s="0" t="n">
+        <f aca="false">AVERAGE(AP34:AP37)</f>
+        <v>48.17433023455</v>
+      </c>
+      <c r="AQ31" s="0" t="n">
+        <f aca="false">AVERAGE(AQ34:AQ37)</f>
+        <v>54.543495059</v>
+      </c>
+      <c r="AR31" s="0" t="n">
+        <f aca="false">AVERAGE(AR34:AR37)</f>
         <v>1034.37035590228</v>
       </c>
     </row>
@@ -4140,61 +5383,92 @@
       </c>
       <c r="T32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(T34:T37)</f>
-        <v>0.35313093591189</v>
+        <v>21.8251957839138</v>
       </c>
       <c r="U32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(U34:U37)</f>
-        <v>1.9651214163548</v>
+        <v>193.643456009775</v>
       </c>
       <c r="V32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(V34:V37)</f>
-        <v>6391.96801832692</v>
+        <v>6383.80550416727</v>
       </c>
       <c r="W32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(W34:W37)</f>
-        <v>1.89282913407949</v>
+        <v>11.030484940839</v>
       </c>
       <c r="X32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(X34:X37)</f>
-        <v>657.713123212753</v>
+        <v>660.045225050365</v>
       </c>
       <c r="Y32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Y34:Y37)</f>
-        <v>8366.82170401625</v>
+        <v>8359.50193601807</v>
       </c>
       <c r="Z32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(Z34:Z37)</f>
-        <v>2.79268360747295</v>
+        <v>623.788601255195</v>
       </c>
       <c r="AB32" s="0" t="s">
         <v>7</v>
       </c>
       <c r="AC32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AC34:AC37)</f>
-        <v>21.9993295830989</v>
+        <v>0.35313093591189</v>
       </c>
       <c r="AD32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AD34:AD37)</f>
-        <v>195.002339362494</v>
+        <v>1.9651214163548</v>
       </c>
       <c r="AE32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AE34:AE37)</f>
-        <v>4.80735591344712</v>
+        <v>6391.96801832692</v>
       </c>
       <c r="AF32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AF34:AF37)</f>
-        <v>11.8334570205585</v>
+        <v>1.89282913407949</v>
       </c>
       <c r="AG32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AG34:AG37)</f>
-        <v>6.49212026156401</v>
+        <v>657.713123212753</v>
       </c>
       <c r="AH32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AH34:AH37)</f>
-        <v>5.97776193720353</v>
+        <v>8366.82170401625</v>
       </c>
       <c r="AI32" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(AI34:AI37)</f>
+        <v>2.79268360747295</v>
+      </c>
+      <c r="AK32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AL34:AL37)</f>
+        <v>21.9993295830989</v>
+      </c>
+      <c r="AM32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AM34:AM37)</f>
+        <v>195.002339362494</v>
+      </c>
+      <c r="AN32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AN34:AN37)</f>
+        <v>4.80735591344712</v>
+      </c>
+      <c r="AO32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AO34:AO37)</f>
+        <v>11.8334570205585</v>
+      </c>
+      <c r="AP32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AP34:AP37)</f>
+        <v>6.49212026156401</v>
+      </c>
+      <c r="AQ32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AQ34:AQ37)</f>
+        <v>5.97776193720353</v>
+      </c>
+      <c r="AR32" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(AR34:AR37)</f>
         <v>609.458721608523</v>
       </c>
     </row>
@@ -4251,48 +5525,79 @@
         <v>8</v>
       </c>
       <c r="T34" s="0" t="n">
-        <v>5.46191000938</v>
+        <f aca="false">B34-K34</f>
+        <v>118.685358043</v>
       </c>
       <c r="U34" s="0" t="n">
-        <v>9.64876389503</v>
+        <f aca="false">C34-L34</f>
+        <v>92.428524732</v>
       </c>
       <c r="V34" s="0" t="n">
-        <v>95.7308750153</v>
+        <f aca="false">D34-M34</f>
+        <v>161.755822184</v>
       </c>
       <c r="W34" s="0" t="n">
-        <v>12.0980529785</v>
+        <f aca="false">E34-N34</f>
+        <v>96.595077037</v>
       </c>
       <c r="X34" s="0" t="n">
-        <v>424.384809971</v>
+        <f aca="false">F34-O34</f>
+        <v>499.658962961</v>
       </c>
       <c r="Y34" s="0" t="n">
-        <v>97.7355091572</v>
+        <f aca="false">G34-P34</f>
+        <v>4817.869013069</v>
       </c>
       <c r="Z34" s="0" t="n">
-        <v>46.1465489864</v>
+        <f aca="false">H34-Q34</f>
+        <v>8788.674225095</v>
       </c>
       <c r="AB34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="AC34" s="0" t="n">
+        <v>5.46191000938</v>
+      </c>
+      <c r="AD34" s="0" t="n">
+        <v>9.64876389503</v>
+      </c>
+      <c r="AE34" s="0" t="n">
+        <v>95.7308750153</v>
+      </c>
+      <c r="AF34" s="0" t="n">
+        <v>12.0980529785</v>
+      </c>
+      <c r="AG34" s="0" t="n">
+        <v>424.384809971</v>
+      </c>
+      <c r="AH34" s="0" t="n">
+        <v>97.7355091572</v>
+      </c>
+      <c r="AI34" s="0" t="n">
+        <v>46.1465489864</v>
+      </c>
+      <c r="AK34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL34" s="0" t="n">
         <v>99.58379888537</v>
       </c>
-      <c r="AD34" s="0" t="n">
+      <c r="AM34" s="0" t="n">
         <v>70.62323594092</v>
       </c>
-      <c r="AE34" s="0" t="n">
+      <c r="AN34" s="0" t="n">
         <v>37.981541872</v>
       </c>
-      <c r="AF34" s="0" t="n">
+      <c r="AO34" s="0" t="n">
         <v>80.5118999481</v>
       </c>
-      <c r="AG34" s="0" t="n">
+      <c r="AP34" s="0" t="n">
         <v>42.1768257618</v>
       </c>
-      <c r="AH34" s="0" t="n">
+      <c r="AQ34" s="0" t="n">
         <v>52.0753657818</v>
       </c>
-      <c r="AI34" s="0" t="n">
+      <c r="AR34" s="0" t="n">
         <v>82.6733875275</v>
       </c>
     </row>
@@ -4349,48 +5654,79 @@
         <v>9</v>
       </c>
       <c r="T35" s="0" t="n">
-        <v>6.42661690712</v>
+        <f aca="false">B35-K35</f>
+        <v>90.282166005</v>
       </c>
       <c r="U35" s="0" t="n">
-        <v>9.10378909111</v>
+        <f aca="false">C35-L35</f>
+        <v>283.883352992</v>
       </c>
       <c r="V35" s="0" t="n">
-        <v>67.0543301105</v>
+        <f aca="false">D35-M35</f>
+        <v>161.546872849</v>
       </c>
       <c r="W35" s="0" t="n">
-        <v>13.7307200432</v>
+        <f aca="false">E35-N35</f>
+        <v>113.688202144</v>
       </c>
       <c r="X35" s="0" t="n">
-        <v>842.088745117</v>
+        <f aca="false">F35-O35</f>
+        <v>927.223453048</v>
       </c>
       <c r="Y35" s="0" t="n">
-        <v>23736.5123549</v>
+        <f aca="false">G35-P35</f>
+        <v>28437.614125028</v>
       </c>
       <c r="Z35" s="0" t="n">
-        <v>39.0618598461</v>
+        <f aca="false">H35-Q35</f>
+        <v>10382.848640185</v>
       </c>
       <c r="AB35" s="0" t="s">
         <v>9</v>
       </c>
       <c r="AC35" s="0" t="n">
+        <v>6.42661690712</v>
+      </c>
+      <c r="AD35" s="0" t="n">
+        <v>9.10378909111</v>
+      </c>
+      <c r="AE35" s="0" t="n">
+        <v>67.0543301105</v>
+      </c>
+      <c r="AF35" s="0" t="n">
+        <v>13.7307200432</v>
+      </c>
+      <c r="AG35" s="0" t="n">
+        <v>842.088745117</v>
+      </c>
+      <c r="AH35" s="0" t="n">
+        <v>23736.5123549</v>
+      </c>
+      <c r="AI35" s="0" t="n">
+        <v>39.0618598461</v>
+      </c>
+      <c r="AK35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL35" s="0" t="n">
         <v>69.57026600839</v>
       </c>
-      <c r="AD35" s="0" t="n">
+      <c r="AM35" s="0" t="n">
         <v>261.61546802504</v>
       </c>
-      <c r="AE35" s="0" t="n">
+      <c r="AN35" s="0" t="n">
         <v>33.2256019115</v>
       </c>
-      <c r="AF35" s="0" t="n">
+      <c r="AO35" s="0" t="n">
         <v>88.1410548687</v>
       </c>
-      <c r="AG35" s="0" t="n">
+      <c r="AP35" s="0" t="n">
         <v>58.7053947449</v>
       </c>
-      <c r="AH35" s="0" t="n">
+      <c r="AQ35" s="0" t="n">
         <v>52.7295157909</v>
       </c>
-      <c r="AI35" s="0" t="n">
+      <c r="AR35" s="0" t="n">
         <v>1637.9518008206</v>
       </c>
     </row>
@@ -4447,48 +5783,79 @@
         <v>10</v>
       </c>
       <c r="T36" s="0" t="n">
-        <v>5.91909813881</v>
+        <f aca="false">B36-K36</f>
+        <v>151.010187151</v>
       </c>
       <c r="U36" s="0" t="n">
-        <v>5.43118309975</v>
+        <f aca="false">C36-L36</f>
+        <v>566.632090089</v>
       </c>
       <c r="V36" s="0" t="n">
-        <v>15247.448909</v>
+        <f aca="false">D36-M36</f>
+        <v>15307.914527152</v>
       </c>
       <c r="W36" s="0" t="n">
-        <v>8.68179917336</v>
+        <f aca="false">E36-N36</f>
+        <v>108.296689986</v>
       </c>
       <c r="X36" s="0" t="n">
-        <v>73.0594861507</v>
+        <f aca="false">F36-O36</f>
+        <v>146.822295902</v>
       </c>
       <c r="Y36" s="0" t="n">
-        <v>11553.2820418</v>
+        <f aca="false">G36-P36</f>
+        <v>16309.722354149</v>
       </c>
       <c r="Z36" s="0" t="n">
-        <v>41.4889578819</v>
+        <f aca="false">H36-Q36</f>
+        <v>9628.478999113</v>
       </c>
       <c r="AB36" s="0" t="s">
         <v>10</v>
       </c>
       <c r="AC36" s="0" t="n">
+        <v>5.91909813881</v>
+      </c>
+      <c r="AD36" s="0" t="n">
+        <v>5.43118309975</v>
+      </c>
+      <c r="AE36" s="0" t="n">
+        <v>15247.448909</v>
+      </c>
+      <c r="AF36" s="0" t="n">
+        <v>8.68179917336</v>
+      </c>
+      <c r="AG36" s="0" t="n">
+        <v>73.0594861507</v>
+      </c>
+      <c r="AH36" s="0" t="n">
+        <v>11553.2820418</v>
+      </c>
+      <c r="AI36" s="0" t="n">
+        <v>41.4889578819</v>
+      </c>
+      <c r="AK36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL36" s="0" t="n">
         <v>131.45075106667</v>
       </c>
-      <c r="AD36" s="0" t="n">
+      <c r="AM36" s="0" t="n">
         <v>551.0800180436</v>
       </c>
-      <c r="AE36" s="0" t="n">
+      <c r="AN36" s="0" t="n">
         <v>39.8868918419</v>
       </c>
-      <c r="AF36" s="0" t="n">
+      <c r="AO36" s="0" t="n">
         <v>94.4419589043</v>
       </c>
-      <c r="AG36" s="0" t="n">
+      <c r="AP36" s="0" t="n">
         <v>48.299258709</v>
       </c>
-      <c r="AH36" s="0" t="n">
+      <c r="AQ36" s="0" t="n">
         <v>64.570744276</v>
       </c>
-      <c r="AI36" s="0" t="n">
+      <c r="AR36" s="0" t="n">
         <v>929.9233202933</v>
       </c>
     </row>
@@ -4545,74 +5912,87 @@
         <v>11</v>
       </c>
       <c r="T37" s="0" t="n">
-        <v>5.72594189644</v>
+        <f aca="false">B37-K37</f>
+        <v>111.134639742</v>
       </c>
       <c r="U37" s="0" t="n">
-        <v>5.49935317039</v>
+        <f aca="false">C37-L37</f>
+        <v>94.716400861</v>
       </c>
       <c r="V37" s="0" t="n">
-        <v>8804.45973492</v>
+        <f aca="false">D37-M37</f>
+        <v>8875.077677016</v>
       </c>
       <c r="W37" s="0" t="n">
-        <v>10.3173758984</v>
+        <f aca="false">E37-N37</f>
+        <v>127.295067075</v>
       </c>
       <c r="X37" s="0" t="n">
-        <v>1829.21795106</v>
+        <f aca="false">F37-O37</f>
+        <v>1908.85872006</v>
       </c>
       <c r="Y37" s="0" t="n">
-        <v>12637.01897</v>
+        <f aca="false">G37-P37</f>
+        <v>17347.557379687</v>
       </c>
       <c r="Z37" s="0" t="n">
-        <v>39.581485033</v>
+        <f aca="false">H37-Q37</f>
+        <v>10215.940354847</v>
       </c>
       <c r="AB37" s="0" t="s">
         <v>11</v>
       </c>
       <c r="AC37" s="0" t="n">
+        <v>5.72594189644</v>
+      </c>
+      <c r="AD37" s="0" t="n">
+        <v>5.49935317039</v>
+      </c>
+      <c r="AE37" s="0" t="n">
+        <v>8804.45973492</v>
+      </c>
+      <c r="AF37" s="0" t="n">
+        <v>10.3173758984</v>
+      </c>
+      <c r="AG37" s="0" t="n">
+        <v>1829.21795106</v>
+      </c>
+      <c r="AH37" s="0" t="n">
+        <v>12637.01897</v>
+      </c>
+      <c r="AI37" s="0" t="n">
+        <v>39.581485033</v>
+      </c>
+      <c r="AK37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL37" s="0" t="n">
         <v>94.94647884365</v>
       </c>
-      <c r="AD37" s="0" t="n">
+      <c r="AM37" s="0" t="n">
         <v>78.20464992522</v>
       </c>
-      <c r="AE37" s="0" t="n">
+      <c r="AN37" s="0" t="n">
         <v>46.6161930561</v>
       </c>
-      <c r="AF37" s="0" t="n">
+      <c r="AO37" s="0" t="n">
         <v>112.5392789838</v>
       </c>
-      <c r="AG37" s="0" t="n">
+      <c r="AP37" s="0" t="n">
         <v>43.5158417225</v>
       </c>
-      <c r="AH37" s="0" t="n">
+      <c r="AQ37" s="0" t="n">
         <v>48.7983543873</v>
       </c>
-      <c r="AI37" s="0" t="n">
+      <c r="AR37" s="0" t="n">
         <v>1486.9329149677</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4629,10 +6009,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="M1:S136"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF11" activeCellId="0" sqref="AF11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C136" activeCellId="0" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4644,27 +6024,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4675,18 +6067,348 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M93" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N93" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O93" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="P93" s="0" t="n">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M95" s="0" t="n">
+        <v>134.391339005</v>
+      </c>
+      <c r="N95" s="0" t="n">
+        <v>117.683530095</v>
+      </c>
+      <c r="O95" s="0" t="n">
+        <v>140.19159406</v>
+      </c>
+      <c r="P95" s="0" t="n">
+        <v>209.6199097075</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M96" s="0" t="n">
+        <v>22.0923253591981</v>
+      </c>
+      <c r="N96" s="0" t="n">
+        <v>4.82326564498172</v>
+      </c>
+      <c r="O96" s="0" t="n">
+        <v>6.23869432135785</v>
+      </c>
+      <c r="P96" s="0" t="n">
+        <v>5.41536815417673</v>
+      </c>
+    </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M98" s="0" t="n">
+        <v>126.00367785</v>
+      </c>
+      <c r="N98" s="0" t="n">
+        <v>113.59935403</v>
+      </c>
+      <c r="O98" s="0" t="n">
+        <v>150.74305105</v>
+      </c>
+      <c r="P98" s="0" t="n">
+        <v>208.54335213</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M99" s="0" t="n">
+        <v>170.7058928</v>
+      </c>
+      <c r="N99" s="0" t="n">
+        <v>113.057899</v>
+      </c>
+      <c r="O99" s="0" t="n">
+        <v>136.32205438</v>
+      </c>
+      <c r="P99" s="0" t="n">
+        <v>218.66549397</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M100" s="0" t="n">
+        <v>129.73455739</v>
+      </c>
+      <c r="N100" s="0" t="n">
+        <v>119.11882425</v>
+      </c>
+      <c r="O100" s="0" t="n">
+        <v>138.72875094</v>
+      </c>
+      <c r="P100" s="0" t="n">
+        <v>206.76910377</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M101" s="0" t="n">
+        <v>111.12122798</v>
+      </c>
+      <c r="N101" s="0" t="n">
+        <v>124.9580431</v>
+      </c>
+      <c r="O101" s="0" t="n">
+        <v>134.97251987</v>
+      </c>
+      <c r="P101" s="0" t="n">
+        <v>204.50168896</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M106" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N106" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O106" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="P106" s="0" t="n">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M108" s="0" t="n">
+        <v>129.40085655175</v>
+      </c>
+      <c r="N108" s="0" t="n">
+        <v>118.0718771795</v>
+      </c>
+      <c r="O108" s="0" t="n">
+        <v>130.57775896725</v>
+      </c>
+      <c r="P108" s="0" t="n">
+        <v>184.78897744</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M109" s="0" t="n">
+        <v>8.30532410306872</v>
+      </c>
+      <c r="N109" s="0" t="n">
+        <v>11.0461881096775</v>
+      </c>
+      <c r="O109" s="0" t="n">
+        <v>9.84240349163049</v>
+      </c>
+      <c r="P109" s="0" t="n">
+        <v>18.2364689097185</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M111" s="0" t="n">
+        <v>119.84542823</v>
+      </c>
+      <c r="N111" s="0" t="n">
+        <v>103.112755778</v>
+      </c>
+      <c r="O111" s="0" t="n">
+        <v>122.231108189</v>
+      </c>
+      <c r="P111" s="0" t="n">
+        <v>160.42066788</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M112" s="0" t="n">
+        <v>135.50799894</v>
+      </c>
+      <c r="N112" s="0" t="n">
+        <v>133.668916937</v>
+      </c>
+      <c r="O112" s="0" t="n">
+        <v>143.33517885</v>
+      </c>
+      <c r="P112" s="0" t="n">
+        <v>176.32802319</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M113" s="0" t="n">
+        <v>122.717714067</v>
+      </c>
+      <c r="N113" s="0" t="n">
+        <v>114.525949238</v>
+      </c>
+      <c r="O113" s="0" t="n">
+        <v>136.89721584</v>
+      </c>
+      <c r="P113" s="0" t="n">
+        <v>209.14063191</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M114" s="0" t="n">
+        <v>139.53228497</v>
+      </c>
+      <c r="N114" s="0" t="n">
+        <v>120.979886765</v>
+      </c>
+      <c r="O114" s="0" t="n">
+        <v>119.84753299</v>
+      </c>
+      <c r="P114" s="0" t="n">
+        <v>193.26658678</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M119" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N119" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O119" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="P119" s="0" t="n">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M121" s="0" t="n">
+        <v>117.77808773525</v>
+      </c>
+      <c r="N121" s="0" t="n">
+        <v>259.4150921685</v>
+      </c>
+      <c r="O121" s="0" t="n">
+        <v>111.4687590605</v>
+      </c>
+      <c r="P121" s="0" t="n">
+        <v>9753.98555481</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M122" s="0" t="n">
+        <v>21.8251957839138</v>
+      </c>
+      <c r="N122" s="0" t="n">
+        <v>193.643456009775</v>
+      </c>
+      <c r="O122" s="0" t="n">
+        <v>11.030484940839</v>
+      </c>
+      <c r="P122" s="0" t="n">
+        <v>623.788601255195</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M124" s="0" t="n">
+        <v>118.685358043</v>
+      </c>
+      <c r="N124" s="0" t="n">
+        <v>92.428524732</v>
+      </c>
+      <c r="O124" s="0" t="n">
+        <v>96.595077037</v>
+      </c>
+      <c r="P124" s="0" t="n">
+        <v>8788.674225095</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M125" s="0" t="n">
+        <v>90.282166005</v>
+      </c>
+      <c r="N125" s="0" t="n">
+        <v>283.883352992</v>
+      </c>
+      <c r="O125" s="0" t="n">
+        <v>113.688202144</v>
+      </c>
+      <c r="P125" s="0" t="n">
+        <v>10382.848640185</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M126" s="0" t="n">
+        <v>151.010187151</v>
+      </c>
+      <c r="N126" s="0" t="n">
+        <v>566.632090089</v>
+      </c>
+      <c r="O126" s="0" t="n">
+        <v>108.296689986</v>
+      </c>
+      <c r="P126" s="0" t="n">
+        <v>9628.478999113</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M127" s="0" t="n">
+        <v>111.134639742</v>
+      </c>
+      <c r="N127" s="0" t="n">
+        <v>94.716400861</v>
+      </c>
+      <c r="O127" s="0" t="n">
+        <v>127.295067075</v>
+      </c>
+      <c r="P127" s="0" t="n">
+        <v>10215.940354847</v>
+      </c>
+    </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4698,4 +6420,311 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:H19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L39" activeCellId="0" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1019.2150266765</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>21.8631076138165</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1708.1714770175</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>389.95321554158</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1939.5044540175</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>21.3459437562951</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1162.7750162465</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>193.755464912202</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1034.898582695</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2.1150456385541</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1922.332989575</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>5.25514853659808</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1022.47398907</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>11.0578391644769</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1591.784653245</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>387.649443187899</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1971.5520235875</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>20.6882619440157</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>10703.97628748</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>622.096870048414</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>3774.58370894</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>115.494131234116</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2835.0577372325</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>625.412181601585</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>117.77808773525</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>21.8251957839138</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>129.40085655175</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>8.30532410306872</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>134.391339005</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>22.0923253591981</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>259.4150921685</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>193.643456009775</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>118.0718771795</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>11.0461881096775</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>117.683530095</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>4.82326564498172</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>111.4687590605</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>11.030484940839</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>130.57775896725</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>9.84240349163049</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>140.19159406</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>6.23869432135785</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>9753.98555481</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>623.788601255195</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>184.78897744</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>18.2364689097185</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>209.6199097075</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>5.41536815417673</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding data about Wait Time per Job by Job Size to Summary File for AIMES Experiment
</commit_message>
<xml_diff>
--- a/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
+++ b/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="45" windowWidth="28005" windowHeight="16440" tabRatio="462"/>
+    <workbookView xWindow="780" yWindow="45" windowWidth="28005" windowHeight="16440" tabRatio="462" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timings_AIMES" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="44">
   <si>
     <t>TTC_AIMES_SWIFT_1_v2</t>
   </si>
@@ -122,12 +122,45 @@
   <si>
     <t>Tw_StDev</t>
   </si>
+  <si>
+    <t>Run 5</t>
+  </si>
+  <si>
+    <t>Run 6</t>
+  </si>
+  <si>
+    <t>Run 7</t>
+  </si>
+  <si>
+    <t>Run 8</t>
+  </si>
+  <si>
+    <t>NOTE: Runs 1-4 are 20 min, but Runs 5-8 are 15 min</t>
+  </si>
+  <si>
+    <t>Stampede</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>**Averaged across all number of Resources</t>
+  </si>
+  <si>
+    <t>Measured**</t>
+  </si>
+  <si>
+    <t>NOTE: XDMoD did not provide Wait Time Per Job for Job Size of less than 9 Cores</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +173,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,9 +202,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,42 +449,42 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$6:$G$9</c:f>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.3459437562951</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.6882619440157</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$6:$G$9</c:f>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.3459437562951</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.6882619440157</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -453,16 +497,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1343.6227599399999</c:v>
+                  <c:v>1525.8971184787499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1355.4074729675001</c:v>
+                  <c:v>1195.15302783125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1487.1671472200001</c:v>
+                  <c:v>1539.4759002325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2331.0594869249999</c:v>
+                  <c:v>3052.8215979325005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,16 +535,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>389.95321554157999</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1150456385541001</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>387.64944318789901</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>115.494131234116</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -512,16 +556,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>389.95321554157999</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1150456385541001</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>387.64944318789901</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>115.494131234116</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -598,11 +642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239383680"/>
-        <c:axId val="239385216"/>
+        <c:axId val="238288256"/>
+        <c:axId val="238560768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239383680"/>
+        <c:axId val="238288256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239385216"/>
+        <c:crossAx val="238560768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239385216"/>
+        <c:axId val="238560768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -632,7 +676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239383680"/>
+        <c:crossAx val="238288256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -927,11 +971,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238306048"/>
-        <c:axId val="238307968"/>
+        <c:axId val="238367872"/>
+        <c:axId val="238369792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238306048"/>
+        <c:axId val="238367872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238307968"/>
+        <c:crossAx val="238369792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1019,7 +1063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238307968"/>
+        <c:axId val="238369792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -1128,7 +1172,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238306048"/>
+        <c:crossAx val="238367872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1360,16 +1404,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5.2901632702800718</c:v>
+                    <c:v>7.0244094563688133</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.931162871998762</c:v>
+                    <c:v>19.305037162582359</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.021244097630778</c:v>
+                    <c:v>55.598549503909751</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>123.55531007138792</c:v>
+                    <c:v>199.55844957340665</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1381,16 +1425,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5.2901632702800718</c:v>
+                    <c:v>7.0244094563688133</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.931162871998762</c:v>
+                    <c:v>19.305037162582359</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.021244097630778</c:v>
+                    <c:v>55.598549503909751</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>123.55531007138792</c:v>
+                    <c:v>199.55844957340665</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1424,16 +1468,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>127.54590612749996</c:v>
+                  <c:v>128.47338133962498</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144.02130383000008</c:v>
+                  <c:v>131.04659050475004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>222.60707020750004</c:v>
+                  <c:v>176.592414587375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>542.69585400750009</c:v>
+                  <c:v>363.74241572375007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,11 +1596,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239404928"/>
-        <c:axId val="239406464"/>
+        <c:axId val="238604672"/>
+        <c:axId val="238606208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239404928"/>
+        <c:axId val="238604672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239406464"/>
+        <c:crossAx val="238606208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1574,7 +1618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239406464"/>
+        <c:axId val="238606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -1586,7 +1630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239404928"/>
+        <c:crossAx val="238604672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -1814,11 +1858,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="162645888"/>
-        <c:axId val="162680832"/>
+        <c:axId val="238910080"/>
+        <c:axId val="238920448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="162645888"/>
+        <c:axId val="238910080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162680832"/>
+        <c:crossAx val="238920448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1836,7 +1880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162680832"/>
+        <c:axId val="238920448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -1848,7 +1892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162645888"/>
+        <c:crossAx val="238910080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -1939,47 +1983,68 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$6:$G$9</c:f>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.3459437562951</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.6882619440157</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$6:$G$9</c:f>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.3459437562951</c:v>
+                    <c:v>330.55075412857184</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>160.49379901294051</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>20.6882619440157</c:v>
+                    <c:v>282.44061723090124</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>734.45939887387738</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Plot Data'!$D$6:$D$9</c:f>
@@ -1987,16 +2052,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1343.6227599399999</c:v>
+                  <c:v>1525.8971184787499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1355.4074729675001</c:v>
+                  <c:v>1195.15302783125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1487.1671472200001</c:v>
+                  <c:v>1539.4759002325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2331.0594869249999</c:v>
+                  <c:v>3052.8215979325005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,6 +2083,27 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Plot Data'!$H$6:$H$9</c:f>
@@ -2051,11 +2137,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="214563072"/>
-        <c:axId val="217162880"/>
+        <c:axId val="239012864"/>
+        <c:axId val="239019136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="214563072"/>
+        <c:axId val="239012864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2065,7 +2151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217162880"/>
+        <c:crossAx val="239019136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2073,7 +2159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217162880"/>
+        <c:axId val="239019136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2085,7 +2171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214563072"/>
+        <c:crossAx val="239012864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2180,47 +2266,68 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Plot Data'!$E$6:$E$10</c:f>
+                <c:f>'Plot Data'!$G$6:$G$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>389.95321554157999</c:v>
+                    <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1150456385541001</c:v>
+                    <c:v>5.2551485365980799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>387.64944318789901</c:v>
+                    <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>115.494131234116</c:v>
+                    <c:v>625.41218160158496</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Plot Data'!$E$6:$E$9</c:f>
+                <c:f>'Plot Data'!$G$6:$G$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>389.95321554157999</c:v>
+                    <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1150456385541001</c:v>
+                    <c:v>5.2551485365980799</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>387.64944318789901</c:v>
+                    <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>115.494131234116</c:v>
+                    <c:v>625.41218160158496</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Plot Data'!$F$6:$F$9</c:f>
@@ -2259,6 +2366,27 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Plot Data'!$H$6:$H$9</c:f>
@@ -2292,11 +2420,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="162437760"/>
-        <c:axId val="162448128"/>
+        <c:axId val="239053056"/>
+        <c:axId val="239055232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="162437760"/>
+        <c:axId val="239053056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,7 +2434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162448128"/>
+        <c:crossAx val="239055232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2314,7 +2442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162448128"/>
+        <c:axId val="239055232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2326,7 +2454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162437760"/>
+        <c:crossAx val="239053056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2517,11 +2645,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="10590848"/>
-        <c:axId val="10613888"/>
+        <c:axId val="239062016"/>
+        <c:axId val="239067904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10590848"/>
+        <c:axId val="239062016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2531,7 +2659,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10613888"/>
+        <c:crossAx val="239067904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2539,7 +2667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10613888"/>
+        <c:axId val="239067904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2551,7 +2679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10590848"/>
+        <c:crossAx val="239062016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2648,16 +2776,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5.2901632702800718</c:v>
+                    <c:v>7.0244094563688133</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.931162871998762</c:v>
+                    <c:v>19.305037162582359</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.021244097630778</c:v>
+                    <c:v>55.598549503909751</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>123.55531007138792</c:v>
+                    <c:v>199.55844957340665</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2669,16 +2797,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>5.2901632702800718</c:v>
+                    <c:v>7.0244094563688133</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>16.931162871998762</c:v>
+                    <c:v>19.305037162582359</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.021244097630778</c:v>
+                    <c:v>55.598549503909751</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>123.55531007138792</c:v>
+                    <c:v>199.55844957340665</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2712,16 +2840,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>127.54590612749996</c:v>
+                  <c:v>128.47338133962498</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144.02130383000008</c:v>
+                  <c:v>131.04659050475004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>222.60707020750004</c:v>
+                  <c:v>176.592414587375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>542.69585400750009</c:v>
+                  <c:v>363.74241572375007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2738,11 +2866,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="10191616"/>
-        <c:axId val="10193152"/>
+        <c:axId val="239125632"/>
+        <c:axId val="239127168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10191616"/>
+        <c:axId val="239125632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,7 +2880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10193152"/>
+        <c:crossAx val="239127168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2760,7 +2888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10193152"/>
+        <c:axId val="239127168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2772,7 +2900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10191616"/>
+        <c:crossAx val="239125632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -2962,11 +3090,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="165791232"/>
-        <c:axId val="165792768"/>
+        <c:axId val="239139840"/>
+        <c:axId val="239158016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165791232"/>
+        <c:axId val="239139840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +3104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165792768"/>
+        <c:crossAx val="239158016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2984,7 +3112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165792768"/>
+        <c:axId val="239158016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2996,7 +3124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165791232"/>
+        <c:crossAx val="239139840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
@@ -3327,11 +3455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239502080"/>
-        <c:axId val="239504384"/>
+        <c:axId val="239228032"/>
+        <c:axId val="239230336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239502080"/>
+        <c:axId val="239228032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,7 +3539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239504384"/>
+        <c:crossAx val="239230336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3419,7 +3547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239504384"/>
+        <c:axId val="239230336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -3528,7 +3656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239502080"/>
+        <c:crossAx val="239228032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5326,7 +5454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5334,10 +5462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR41"/>
+  <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14:Z24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z18" activeCellId="2" sqref="T18:U19 W18:W19 Z18:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6493,20 +6621,20 @@
         <v>6</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:H18" si="11">AVERAGE(B21:B24)</f>
-        <v>1343.6227599399999</v>
+        <f>AVERAGE(B21:B28)</f>
+        <v>1525.8971184787499</v>
       </c>
       <c r="C18">
-        <f t="shared" si="11"/>
-        <v>1355.4074729675001</v>
+        <f>AVERAGE(C21:C28)</f>
+        <v>1195.15302783125</v>
       </c>
       <c r="D18">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="D18:G18" si="11">AVERAGE(D21:D24)</f>
         <v>4209.7526777375006</v>
       </c>
       <c r="E18">
-        <f t="shared" si="11"/>
-        <v>1487.1671472200001</v>
+        <f>AVERAGE(E21:E28)</f>
+        <v>1539.4759002325</v>
       </c>
       <c r="F18">
         <f t="shared" si="11"/>
@@ -6517,27 +6645,27 @@
         <v>4331.6253030299995</v>
       </c>
       <c r="H18">
-        <f t="shared" si="11"/>
-        <v>2331.0594869249999</v>
+        <f>AVERAGE(H21:H28)</f>
+        <v>3052.8215979325005</v>
       </c>
       <c r="J18" t="s">
         <v>6</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:Q18" si="12">AVERAGE(K21:K24)</f>
-        <v>1216.0768538124998</v>
+        <f>AVERAGE(K21:K28)</f>
+        <v>1397.4237371391248</v>
       </c>
       <c r="L18">
-        <f t="shared" si="12"/>
-        <v>1211.3861691375</v>
+        <f>AVERAGE(L21:L28)</f>
+        <v>1064.1064373264999</v>
       </c>
       <c r="M18">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="M18:P18" si="12">AVERAGE(M21:M24)</f>
         <v>1925.2562512775</v>
       </c>
       <c r="N18">
-        <f t="shared" si="12"/>
-        <v>1264.5600770125</v>
+        <f>AVERAGE(N21:N28)</f>
+        <v>1362.8834856451251</v>
       </c>
       <c r="O18">
         <f t="shared" si="12"/>
@@ -6548,69 +6676,69 @@
         <v>3094.2151147099999</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="12"/>
-        <v>1788.3636329174999</v>
+        <f>AVERAGE(Q21:Q28)</f>
+        <v>2689.0791822087499</v>
       </c>
       <c r="S18" t="s">
         <v>6</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18:Z18" si="13">AVERAGE(T21:T24)</f>
-        <v>127.54590612749996</v>
+        <f t="shared" ref="T18:U18" si="13">AVERAGE(T21:T28)</f>
+        <v>128.47338133962498</v>
       </c>
       <c r="U18">
         <f t="shared" si="13"/>
-        <v>144.02130383000008</v>
+        <v>131.04659050475004</v>
       </c>
       <c r="V18">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="V18:Y18" si="14">AVERAGE(V21:V24)</f>
         <v>2284.4964264600003</v>
       </c>
       <c r="W18">
-        <f t="shared" si="13"/>
-        <v>222.60707020750004</v>
+        <f>AVERAGE(W21:W28)</f>
+        <v>176.592414587375</v>
       </c>
       <c r="X18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7695.8659844274998</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1237.4101883200001</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="13"/>
-        <v>542.69585400750009</v>
+        <f>AVERAGE(Z21:Z28)</f>
+        <v>363.74241572375007</v>
       </c>
       <c r="AB18" t="s">
         <v>6</v>
       </c>
       <c r="AC18">
-        <f t="shared" ref="AC18:AI18" si="14">AVERAGE(AC21:AC24)</f>
+        <f t="shared" ref="AC18:AI18" si="15">AVERAGE(AC21:AC24)</f>
         <v>12.921206295492501</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17.896859526650001</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2179.2879877079999</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>20.161033988025</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7573.1237204575</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1108.4106562142499</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>88.317779183399992</v>
       </c>
       <c r="AK18" t="s">
@@ -6638,124 +6766,124 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:H19" si="15">_xlfn.STDEV.P(B21:B24)</f>
-        <v>4.0259455151458834</v>
+        <f>_xlfn.STDEV.P(B21:B28)</f>
+        <v>330.55075412857184</v>
       </c>
       <c r="C19">
-        <f t="shared" si="15"/>
-        <v>12.209473915963541</v>
+        <f>_xlfn.STDEV.P(C21:C28)</f>
+        <v>160.49379901294051</v>
       </c>
       <c r="D19">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="D19:G19" si="16">_xlfn.STDEV.P(D21:D24)</f>
         <v>1576.2977787151106</v>
       </c>
       <c r="E19">
-        <f t="shared" si="15"/>
-        <v>61.651459319401468</v>
+        <f>_xlfn.STDEV.P(E21:E28)</f>
+        <v>282.44061723090124</v>
       </c>
       <c r="F19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6229.6303394528959</v>
       </c>
       <c r="G19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>710.40617332203283</v>
       </c>
       <c r="H19">
-        <f t="shared" si="15"/>
-        <v>153.75705859189762</v>
+        <f>_xlfn.STDEV.P(H21:H28)</f>
+        <v>734.45939887387738</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:Q19" si="16">_xlfn.STDEV.P(K21:K24)</f>
-        <v>2.4526346977678104</v>
+        <f>_xlfn.STDEV.P(K21:K28)</f>
+        <v>327.71321001623056</v>
       </c>
       <c r="L19">
-        <f t="shared" si="16"/>
-        <v>7.9028375438364895</v>
+        <f>_xlfn.STDEV.P(L21:L28)</f>
+        <v>147.53325469735103</v>
       </c>
       <c r="M19">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="M19:P19" si="17">_xlfn.STDEV.P(M21:M24)</f>
         <v>31.629008821902389</v>
       </c>
       <c r="N19">
-        <f t="shared" si="16"/>
-        <v>20.841995228746519</v>
+        <f>_xlfn.STDEV.P(N21:N28)</f>
+        <v>289.95656551084716</v>
       </c>
       <c r="O19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>38.306919063538928</v>
       </c>
       <c r="P19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>138.46088687380123</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="16"/>
-        <v>71.384918453766673</v>
+        <f>_xlfn.STDEV.P(Q21:Q28)</f>
+        <v>905.00942414686119</v>
       </c>
       <c r="S19" t="s">
         <v>7</v>
       </c>
       <c r="T19">
-        <f t="shared" ref="T19:Z19" si="17">_xlfn.STDEV.P(T21:T24)</f>
-        <v>5.2901632702800718</v>
+        <f t="shared" ref="T19:U19" si="18">_xlfn.STDEV.P(T21:T28)</f>
+        <v>7.0244094563688133</v>
       </c>
       <c r="U19">
-        <f t="shared" si="17"/>
-        <v>16.931162871998762</v>
+        <f t="shared" si="18"/>
+        <v>19.305037162582359</v>
       </c>
       <c r="V19">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="V19:Y19" si="19">_xlfn.STDEV.P(V21:V24)</f>
         <v>1555.6388055644859</v>
       </c>
       <c r="W19">
-        <f t="shared" si="17"/>
-        <v>43.021244097630778</v>
+        <f>_xlfn.STDEV.P(W21:W28)</f>
+        <v>55.598549503909751</v>
       </c>
       <c r="X19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6214.2089655644522</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>795.45419750778194</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="17"/>
-        <v>123.55531007138792</v>
+        <f>_xlfn.STDEV.P(Z21:Z28)</f>
+        <v>199.55844957340665</v>
       </c>
       <c r="AB19" t="s">
         <v>7</v>
       </c>
       <c r="AC19">
-        <f t="shared" ref="AC19:AI19" si="18">_xlfn.STDEV.P(AC21:AC24)</f>
+        <f t="shared" ref="AC19:AI19" si="20">_xlfn.STDEV.P(AC21:AC24)</f>
         <v>2.3784676023257423</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>6.8563026336923318</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1561.0172793694626</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.6243036679377933</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>6214.9362823004085</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>789.83271678660947</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>4.0259959444986588</v>
       </c>
       <c r="AK19" t="s">
@@ -6831,31 +6959,31 @@
         <v>8</v>
       </c>
       <c r="T21">
-        <f t="shared" ref="T21:Z24" si="19">B21-K21</f>
+        <f t="shared" ref="T21:Z28" si="21">B21-K21</f>
         <v>132.18388389999996</v>
       </c>
       <c r="U21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>135.20589231999998</v>
       </c>
       <c r="V21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1281.3277768999999</v>
       </c>
       <c r="W21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>267.06363106000003</v>
       </c>
       <c r="X21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>7185.0689823600005</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2206.5069041300003</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>751.57537603000014</v>
       </c>
       <c r="AB21" t="s">
@@ -6951,31 +7079,31 @@
         <v>9</v>
       </c>
       <c r="T22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>121.96454000999984</v>
       </c>
       <c r="U22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>135.27315902000009</v>
       </c>
       <c r="V22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>807.45179510999992</v>
       </c>
       <c r="W22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>185.78652978000014</v>
       </c>
       <c r="X22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>948.49650216000009</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>193.90969825000002</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>452.73850798000012</v>
       </c>
       <c r="AB22" t="s">
@@ -7071,31 +7199,31 @@
         <v>10</v>
       </c>
       <c r="T23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>122.59377169999993</v>
       </c>
       <c r="U23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>173.27472496000019</v>
       </c>
       <c r="V23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2217.6387920300003</v>
       </c>
       <c r="W23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>263.74469018000013</v>
       </c>
       <c r="X23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>17741.224369</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1774.7019889400003</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>449.54917716999989</v>
       </c>
       <c r="AB23" t="s">
@@ -7191,31 +7319,31 @@
         <v>11</v>
       </c>
       <c r="T24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>133.44142890000012</v>
       </c>
       <c r="U24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>132.33143902000006</v>
       </c>
       <c r="V24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4831.5673417999997</v>
       </c>
       <c r="W24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>173.83342980999987</v>
       </c>
       <c r="X24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4908.6740841899991</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>774.52216195999972</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>516.92035485000019</v>
       </c>
       <c r="AB24" t="s">
@@ -7256,991 +7384,1200 @@
       </c>
       <c r="AR24">
         <v>2455.6420056850002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>1921.20090413</v>
+      </c>
+      <c r="C25">
+        <v>1033.69503093</v>
+      </c>
+      <c r="E25">
+        <v>1063.6944260600001</v>
+      </c>
+      <c r="H25">
+        <v>3574.62415504</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25">
+        <v>1801.3554759000001</v>
+      </c>
+      <c r="L25">
+        <v>930.58227515199997</v>
+      </c>
+      <c r="N25">
+        <v>941.46331787099996</v>
+      </c>
+      <c r="Q25">
+        <v>3414.2034871599999</v>
+      </c>
+      <c r="S25" t="s">
+        <v>33</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="21"/>
+        <v>119.84542822999992</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="21"/>
+        <v>103.11275577800006</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="21"/>
+        <v>122.23110818900011</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="21"/>
+        <v>160.42066788000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>1937.00067496</v>
+      </c>
+      <c r="C26">
+        <v>1038.4393508400001</v>
+      </c>
+      <c r="E26">
+        <v>1970.65190792</v>
+      </c>
+      <c r="H26">
+        <v>3843.0995960199998</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26">
+        <v>1801.4926760200001</v>
+      </c>
+      <c r="L26">
+        <v>904.77043390300003</v>
+      </c>
+      <c r="N26">
+        <v>1827.3167290700001</v>
+      </c>
+      <c r="Q26">
+        <v>3666.77157283</v>
+      </c>
+      <c r="S26" t="s">
+        <v>34</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="21"/>
+        <v>135.50799893999988</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="21"/>
+        <v>133.66891693700006</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="21"/>
+        <v>143.33517884999992</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="21"/>
+        <v>176.32802318999984</v>
       </c>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>1032.87987494</v>
+      </c>
+      <c r="C27">
+        <v>1032.9629001599999</v>
+      </c>
+      <c r="E27">
+        <v>1376.97004294</v>
+      </c>
+      <c r="H27">
+        <v>3844.69921088</v>
+      </c>
+      <c r="J27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27">
+        <v>910.16216087299995</v>
+      </c>
+      <c r="L27">
+        <v>918.43695092200005</v>
+      </c>
+      <c r="N27">
+        <v>1240.0728271</v>
+      </c>
+      <c r="Q27">
+        <v>3635.5585789699999</v>
+      </c>
+      <c r="S27" t="s">
+        <v>35</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="21"/>
+        <v>122.71771406700009</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="21"/>
+        <v>114.52594923799984</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="21"/>
+        <v>136.89721583999994</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="21"/>
+        <v>209.14063191000014</v>
+      </c>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1941.6044540400001</v>
+      </c>
+      <c r="C28">
+        <v>1034.4970488500001</v>
+      </c>
+      <c r="E28">
+        <v>1955.82223606</v>
+      </c>
+      <c r="H28">
+        <v>3835.91187382</v>
+      </c>
+      <c r="J28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28">
+        <v>1802.07216907</v>
+      </c>
+      <c r="L28">
+        <v>913.517162085</v>
+      </c>
+      <c r="N28">
+        <v>1835.97470307</v>
+      </c>
+      <c r="Q28">
+        <v>3642.6452870399999</v>
+      </c>
+      <c r="S28" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="21"/>
+        <v>139.53228497000009</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="21"/>
+        <v>120.97988676500006</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="21"/>
+        <v>119.84753298999999</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="21"/>
+        <v>193.26658678000013</v>
+      </c>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J33" t="s">
         <v>19</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L33" t="s">
         <v>18</v>
       </c>
-      <c r="S27" t="s">
+      <c r="S33" t="s">
         <v>20</v>
       </c>
-      <c r="U27" t="s">
+      <c r="U33" t="s">
         <v>21</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AB33" t="s">
         <v>20</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AD33" t="s">
         <v>18</v>
       </c>
-      <c r="AK27" t="s">
+      <c r="AK33" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>32</v>
-      </c>
-      <c r="D29">
-        <v>128</v>
-      </c>
-      <c r="E29">
-        <v>256</v>
-      </c>
-      <c r="F29">
-        <v>512</v>
-      </c>
-      <c r="G29">
-        <v>1024</v>
-      </c>
-      <c r="H29">
-        <v>2048</v>
-      </c>
-      <c r="J29" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29">
-        <v>8</v>
-      </c>
-      <c r="L29">
-        <v>32</v>
-      </c>
-      <c r="M29">
-        <v>128</v>
-      </c>
-      <c r="N29">
-        <v>256</v>
-      </c>
-      <c r="O29">
-        <v>512</v>
-      </c>
-      <c r="P29">
-        <v>1024</v>
-      </c>
-      <c r="Q29">
-        <v>2048</v>
-      </c>
-      <c r="S29" t="s">
-        <v>5</v>
-      </c>
-      <c r="T29">
-        <v>8</v>
-      </c>
-      <c r="U29">
-        <v>32</v>
-      </c>
-      <c r="V29">
-        <v>128</v>
-      </c>
-      <c r="W29">
-        <v>256</v>
-      </c>
-      <c r="X29">
-        <v>512</v>
-      </c>
-      <c r="Y29">
-        <v>1024</v>
-      </c>
-      <c r="Z29">
-        <v>2048</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC29">
-        <v>8</v>
-      </c>
-      <c r="AD29">
-        <v>32</v>
-      </c>
-      <c r="AE29">
-        <v>128</v>
-      </c>
-      <c r="AF29">
-        <v>256</v>
-      </c>
-      <c r="AG29">
-        <v>512</v>
-      </c>
-      <c r="AH29">
-        <v>1024</v>
-      </c>
-      <c r="AI29">
-        <v>2048</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL29">
-        <v>8</v>
-      </c>
-      <c r="AM29">
-        <v>32</v>
-      </c>
-      <c r="AN29">
-        <v>128</v>
-      </c>
-      <c r="AO29">
-        <v>256</v>
-      </c>
-      <c r="AP29">
-        <v>512</v>
-      </c>
-      <c r="AQ29">
-        <v>1024</v>
-      </c>
-      <c r="AR29">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <f t="shared" ref="B31:H31" si="20">AVERAGE(B34:B37)</f>
-        <v>1019.2150266765</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="20"/>
-        <v>1162.7750162465002</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="20"/>
-        <v>7031.8574805200005</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="20"/>
-        <v>1022.47398907</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="20"/>
-        <v>1780.6290789825002</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="20"/>
-        <v>17645.6020465375</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="20"/>
-        <v>10703.97628748</v>
-      </c>
-      <c r="J31" t="s">
-        <v>6</v>
-      </c>
-      <c r="K31">
-        <f t="shared" ref="K31:Q31" si="21">AVERAGE(K34:K37)</f>
-        <v>901.43693894124999</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="21"/>
-        <v>903.35992407800006</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="21"/>
-        <v>905.28375571975005</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="21"/>
-        <v>911.0052300095</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="21"/>
-        <v>909.98822098975006</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="21"/>
-        <v>917.41132855425008</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="21"/>
-        <v>949.99073266999994</v>
-      </c>
-      <c r="S31" t="s">
-        <v>6</v>
-      </c>
-      <c r="T31">
-        <f t="shared" ref="T31:Z31" si="22">AVERAGE(T34:T37)</f>
-        <v>117.77808773525004</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="22"/>
-        <v>259.4150921685</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="22"/>
-        <v>6126.5737248002497</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="22"/>
-        <v>111.46875906049999</v>
-      </c>
-      <c r="X31">
-        <f t="shared" si="22"/>
-        <v>870.64085799274994</v>
-      </c>
-      <c r="Y31">
-        <f t="shared" si="22"/>
-        <v>16728.190717983249</v>
-      </c>
-      <c r="Z31">
-        <f t="shared" si="22"/>
-        <v>9753.9855548100004</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" ref="AC31:AI31" si="23">AVERAGE(AC34:AC37)</f>
-        <v>5.8833917379374991</v>
-      </c>
-      <c r="AD31">
-        <f t="shared" si="23"/>
-        <v>7.4207723140699997</v>
-      </c>
-      <c r="AE31">
-        <f t="shared" si="23"/>
-        <v>6053.6734622614495</v>
-      </c>
-      <c r="AF31">
-        <f t="shared" si="23"/>
-        <v>11.206987023365</v>
-      </c>
-      <c r="AG31">
-        <f t="shared" si="23"/>
-        <v>792.18774807467503</v>
-      </c>
-      <c r="AH31">
-        <f t="shared" si="23"/>
-        <v>12006.137218964299</v>
-      </c>
-      <c r="AI31">
-        <f t="shared" si="23"/>
-        <v>41.569712936850003</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL31">
-        <f t="shared" ref="AL31:AR31" si="24">AVERAGE(AL34:AL37)</f>
-        <v>98.887823701019983</v>
-      </c>
-      <c r="AM31">
-        <f t="shared" si="24"/>
-        <v>240.380842983695</v>
-      </c>
-      <c r="AN31">
-        <f t="shared" si="24"/>
-        <v>39.427557170375003</v>
-      </c>
-      <c r="AO31">
-        <f t="shared" si="24"/>
-        <v>93.908548176224997</v>
-      </c>
-      <c r="AP31">
-        <f t="shared" si="24"/>
-        <v>48.174330234549998</v>
-      </c>
-      <c r="AQ31">
-        <f t="shared" si="24"/>
-        <v>54.543495059000001</v>
-      </c>
-      <c r="AR31">
-        <f t="shared" si="24"/>
-        <v>1034.3703559022752</v>
-      </c>
-    </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32">
-        <f t="shared" ref="B32:H32" si="25">_xlfn.STDEV.P(B34:B37)</f>
-        <v>21.863107613816457</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="25"/>
-        <v>193.75546491220152</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="25"/>
-        <v>6383.3760185485135</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="25"/>
-        <v>11.057839164476862</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="25"/>
-        <v>659.77172602622034</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="25"/>
-        <v>8357.0017550937537</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="25"/>
-        <v>622.09687004841385</v>
-      </c>
-      <c r="J32" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32">
-        <f t="shared" ref="K32:Q32" si="26">_xlfn.STDEV.P(K34:K37)</f>
-        <v>0.11143815192325279</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="26"/>
-        <v>0.22979448905687444</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="26"/>
-        <v>1.0908528333074596</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="26"/>
-        <v>0.16820638644878191</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="26"/>
-        <v>0.86373364660478902</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="26"/>
-        <v>2.9439025499627913</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="26"/>
-        <v>4.3118167796588809</v>
-      </c>
-      <c r="S32" t="s">
-        <v>7</v>
-      </c>
-      <c r="T32">
-        <f t="shared" ref="T32:Z32" si="27">_xlfn.STDEV.P(T34:T37)</f>
-        <v>21.825195783913781</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="27"/>
-        <v>193.64345600977541</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="27"/>
-        <v>6383.8055041672733</v>
-      </c>
-      <c r="W32">
-        <f t="shared" si="27"/>
-        <v>11.030484940839022</v>
-      </c>
-      <c r="X32">
-        <f t="shared" si="27"/>
-        <v>660.04522505036482</v>
-      </c>
-      <c r="Y32">
-        <f t="shared" si="27"/>
-        <v>8359.5019360180686</v>
-      </c>
-      <c r="Z32">
-        <f t="shared" si="27"/>
-        <v>623.78860125519509</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" ref="AC32:AI32" si="28">_xlfn.STDEV.P(AC34:AC37)</f>
-        <v>0.35313093591188971</v>
-      </c>
-      <c r="AD32">
-        <f t="shared" si="28"/>
-        <v>1.9651214163548025</v>
-      </c>
-      <c r="AE32">
-        <f t="shared" si="28"/>
-        <v>6391.9680183269165</v>
-      </c>
-      <c r="AF32">
-        <f t="shared" si="28"/>
-        <v>1.8928291340794865</v>
-      </c>
-      <c r="AG32">
-        <f t="shared" si="28"/>
-        <v>657.71312321275275</v>
-      </c>
-      <c r="AH32">
-        <f t="shared" si="28"/>
-        <v>8366.8217040162563</v>
-      </c>
-      <c r="AI32">
-        <f t="shared" si="28"/>
-        <v>2.79268360747295</v>
-      </c>
-      <c r="AK32" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL32">
-        <f t="shared" ref="AL32:AR32" si="29">_xlfn.STDEV.P(AL34:AL37)</f>
-        <v>21.999329583098906</v>
-      </c>
-      <c r="AM32">
-        <f t="shared" si="29"/>
-        <v>195.00233936249393</v>
-      </c>
-      <c r="AN32">
-        <f t="shared" si="29"/>
-        <v>4.8073559134471058</v>
-      </c>
-      <c r="AO32">
-        <f t="shared" si="29"/>
-        <v>11.833457020558477</v>
-      </c>
-      <c r="AP32">
-        <f t="shared" si="29"/>
-        <v>6.4921202615640254</v>
-      </c>
-      <c r="AQ32">
-        <f t="shared" si="29"/>
-        <v>5.9777619372035273</v>
-      </c>
-      <c r="AR32">
-        <f t="shared" si="29"/>
-        <v>609.45872160852252</v>
-      </c>
-    </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34">
-        <v>1020.21847486</v>
-      </c>
-      <c r="C34">
-        <v>995.70735382999999</v>
-      </c>
-      <c r="D34">
-        <v>1068.9020290399999</v>
-      </c>
-      <c r="E34">
-        <v>1007.61050105</v>
-      </c>
-      <c r="F34">
-        <v>1408.5530149900001</v>
-      </c>
-      <c r="G34">
-        <v>5739.4192831500004</v>
-      </c>
-      <c r="H34">
-        <v>9739.9945700200005</v>
-      </c>
-      <c r="J34" t="s">
-        <v>8</v>
-      </c>
-      <c r="K34">
-        <v>901.53311681699995</v>
-      </c>
-      <c r="L34">
-        <v>903.27882909799996</v>
-      </c>
-      <c r="M34">
-        <v>907.14620685600005</v>
-      </c>
-      <c r="N34">
-        <v>911.01542401300003</v>
-      </c>
-      <c r="O34">
-        <v>908.89405202900002</v>
-      </c>
-      <c r="P34">
-        <v>921.55027008100001</v>
-      </c>
-      <c r="Q34">
-        <v>951.32034492499997</v>
-      </c>
-      <c r="S34" t="s">
-        <v>8</v>
-      </c>
-      <c r="T34">
-        <f t="shared" ref="T34:Z37" si="30">B34-K34</f>
-        <v>118.68535804300006</v>
-      </c>
-      <c r="U34">
-        <f t="shared" si="30"/>
-        <v>92.428524732000028</v>
-      </c>
-      <c r="V34">
-        <f t="shared" si="30"/>
-        <v>161.75582218399984</v>
-      </c>
-      <c r="W34">
-        <f t="shared" si="30"/>
-        <v>96.59507703700001</v>
-      </c>
-      <c r="X34">
-        <f t="shared" si="30"/>
-        <v>499.65896296100004</v>
-      </c>
-      <c r="Y34">
-        <f t="shared" si="30"/>
-        <v>4817.8690130690002</v>
-      </c>
-      <c r="Z34">
-        <f t="shared" si="30"/>
-        <v>8788.674225095001</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC34">
-        <v>5.4619100093800004</v>
-      </c>
-      <c r="AD34">
-        <v>9.6487638950299992</v>
-      </c>
-      <c r="AE34">
-        <v>95.730875015300001</v>
-      </c>
-      <c r="AF34">
-        <v>12.0980529785</v>
-      </c>
-      <c r="AG34">
-        <v>424.38480997099998</v>
-      </c>
-      <c r="AH34">
-        <v>97.735509157199999</v>
-      </c>
-      <c r="AI34">
-        <v>46.146548986399999</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL34">
-        <v>99.583798885370001</v>
-      </c>
-      <c r="AM34">
-        <v>70.623235940919997</v>
-      </c>
-      <c r="AN34">
-        <v>37.981541872000001</v>
-      </c>
-      <c r="AO34">
-        <v>80.511899948099995</v>
-      </c>
-      <c r="AP34">
-        <v>42.176825761800004</v>
-      </c>
-      <c r="AQ34">
-        <v>52.075365781800002</v>
-      </c>
-      <c r="AR34">
-        <v>82.673387527499997</v>
       </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>991.73621797600003</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>1186.92613506</v>
+        <v>32</v>
       </c>
       <c r="D35">
-        <v>1065.91628098</v>
+        <v>128</v>
       </c>
       <c r="E35">
-        <v>1024.92551613</v>
+        <v>256</v>
       </c>
       <c r="F35">
-        <v>1838.1210520300001</v>
+        <v>512</v>
       </c>
       <c r="G35">
-        <v>29352.296446100001</v>
+        <v>1024</v>
       </c>
       <c r="H35">
-        <v>11334.252119999999</v>
+        <v>2048</v>
       </c>
       <c r="J35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K35">
-        <v>901.45405197100001</v>
+        <v>8</v>
       </c>
       <c r="L35">
-        <v>903.04278206799995</v>
+        <v>32</v>
       </c>
       <c r="M35">
-        <v>904.369408131</v>
+        <v>128</v>
       </c>
       <c r="N35">
-        <v>911.237313986</v>
+        <v>256</v>
       </c>
       <c r="O35">
-        <v>910.89759898199998</v>
+        <v>512</v>
       </c>
       <c r="P35">
-        <v>914.68232107200004</v>
+        <v>1024</v>
       </c>
       <c r="Q35">
-        <v>951.40347981499997</v>
+        <v>2048</v>
       </c>
       <c r="S35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T35">
-        <f t="shared" si="30"/>
-        <v>90.282166005000022</v>
+        <v>8</v>
       </c>
       <c r="U35">
-        <f t="shared" si="30"/>
-        <v>283.88335299200003</v>
+        <v>32</v>
       </c>
       <c r="V35">
-        <f t="shared" si="30"/>
-        <v>161.54687284900001</v>
+        <v>128</v>
       </c>
       <c r="W35">
-        <f t="shared" si="30"/>
-        <v>113.688202144</v>
+        <v>256</v>
       </c>
       <c r="X35">
-        <f t="shared" si="30"/>
-        <v>927.22345304800012</v>
+        <v>512</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="30"/>
-        <v>28437.614125028002</v>
+        <v>1024</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="30"/>
-        <v>10382.848640184999</v>
+        <v>2048</v>
       </c>
       <c r="AB35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AC35">
-        <v>6.4266169071199997</v>
+        <v>8</v>
       </c>
       <c r="AD35">
-        <v>9.1037890911100003</v>
+        <v>32</v>
       </c>
       <c r="AE35">
-        <v>67.054330110500004</v>
+        <v>128</v>
       </c>
       <c r="AF35">
-        <v>13.7307200432</v>
+        <v>256</v>
       </c>
       <c r="AG35">
-        <v>842.08874511700003</v>
+        <v>512</v>
       </c>
       <c r="AH35">
-        <v>23736.512354900002</v>
+        <v>1024</v>
       </c>
       <c r="AI35">
-        <v>39.061859846099999</v>
+        <v>2048</v>
       </c>
       <c r="AK35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AL35">
-        <v>69.570266008390007</v>
+        <v>8</v>
       </c>
       <c r="AM35">
-        <v>261.61546802504</v>
+        <v>32</v>
       </c>
       <c r="AN35">
-        <v>33.2256019115</v>
+        <v>128</v>
       </c>
       <c r="AO35">
-        <v>88.141054868699996</v>
+        <v>256</v>
       </c>
       <c r="AP35">
-        <v>58.705394744899998</v>
+        <v>512</v>
       </c>
       <c r="AQ35">
-        <v>52.729515790900003</v>
+        <v>1024</v>
       </c>
       <c r="AR35">
-        <v>1637.9518008206001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36">
-        <v>1052.5203139800001</v>
-      </c>
-      <c r="C36">
-        <v>1470.3024210900001</v>
-      </c>
-      <c r="D36">
-        <v>16212.7773051</v>
-      </c>
-      <c r="E36">
-        <v>1019.05859804</v>
-      </c>
-      <c r="F36">
-        <v>1057.5895328500001</v>
-      </c>
-      <c r="G36">
-        <v>17228.561082100001</v>
-      </c>
-      <c r="H36">
-        <v>10582.879688000001</v>
-      </c>
-      <c r="J36" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36">
-        <v>901.510126829</v>
-      </c>
-      <c r="L36">
-        <v>903.67033100100002</v>
-      </c>
-      <c r="M36">
-        <v>904.86277794800003</v>
-      </c>
-      <c r="N36">
-        <v>910.76190805399995</v>
-      </c>
-      <c r="O36">
-        <v>910.767236948</v>
-      </c>
-      <c r="P36">
-        <v>918.83872795100001</v>
-      </c>
-      <c r="Q36">
-        <v>954.400688887</v>
-      </c>
-      <c r="S36" t="s">
-        <v>10</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="30"/>
-        <v>151.01018715100008</v>
-      </c>
-      <c r="U36">
-        <f t="shared" si="30"/>
-        <v>566.63209008900003</v>
-      </c>
-      <c r="V36">
-        <f t="shared" si="30"/>
-        <v>15307.914527152001</v>
-      </c>
-      <c r="W36">
-        <f t="shared" si="30"/>
-        <v>108.29668998600005</v>
-      </c>
-      <c r="X36">
-        <f t="shared" si="30"/>
-        <v>146.82229590200006</v>
-      </c>
-      <c r="Y36">
-        <f t="shared" si="30"/>
-        <v>16309.722354149</v>
-      </c>
-      <c r="Z36">
-        <f t="shared" si="30"/>
-        <v>9628.4789991130001</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC36">
-        <v>5.9190981388099999</v>
-      </c>
-      <c r="AD36">
-        <v>5.4311830997500001</v>
-      </c>
-      <c r="AE36">
-        <v>15247.448909000001</v>
-      </c>
-      <c r="AF36">
-        <v>8.68179917336</v>
-      </c>
-      <c r="AG36">
-        <v>73.059486150699996</v>
-      </c>
-      <c r="AH36">
-        <v>11553.282041799999</v>
-      </c>
-      <c r="AI36">
-        <v>41.488957881899999</v>
-      </c>
-      <c r="AK36" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL36">
-        <v>131.45075106666999</v>
-      </c>
-      <c r="AM36">
-        <v>551.08001804360003</v>
-      </c>
-      <c r="AN36">
-        <v>39.886891841900002</v>
-      </c>
-      <c r="AO36">
-        <v>94.441958904299995</v>
-      </c>
-      <c r="AP36">
-        <v>48.299258709</v>
-      </c>
-      <c r="AQ36">
-        <v>64.570744275999999</v>
-      </c>
-      <c r="AR36">
-        <v>929.92332029329998</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <v>1012.38509989</v>
+        <f t="shared" ref="B37:H37" si="22">AVERAGE(B40:B43)</f>
+        <v>1019.2150266765</v>
       </c>
       <c r="C37">
-        <v>998.16415500599999</v>
+        <f t="shared" si="22"/>
+        <v>1162.7750162465002</v>
       </c>
       <c r="D37">
-        <v>9779.8343069599996</v>
+        <f t="shared" si="22"/>
+        <v>7031.8574805200005</v>
       </c>
       <c r="E37">
-        <v>1038.3013410599999</v>
+        <f t="shared" si="22"/>
+        <v>1022.47398907</v>
       </c>
       <c r="F37">
-        <v>2818.2527160599998</v>
+        <f t="shared" si="22"/>
+        <v>1780.6290789825002</v>
       </c>
       <c r="G37">
-        <v>18262.131374799999</v>
+        <f t="shared" si="22"/>
+        <v>17645.6020465375</v>
       </c>
       <c r="H37">
-        <v>11158.778771900001</v>
+        <f t="shared" si="22"/>
+        <v>10703.97628748</v>
       </c>
       <c r="J37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K37">
-        <v>901.250460148</v>
+        <f t="shared" ref="K37:Q37" si="23">AVERAGE(K40:K43)</f>
+        <v>901.43693894124999</v>
       </c>
       <c r="L37">
-        <v>903.44775414499998</v>
+        <f t="shared" si="23"/>
+        <v>903.35992407800006</v>
       </c>
       <c r="M37">
-        <v>904.756629944</v>
+        <f t="shared" si="23"/>
+        <v>905.28375571975005</v>
       </c>
       <c r="N37">
-        <v>911.00627398500001</v>
+        <f t="shared" si="23"/>
+        <v>911.0052300095</v>
       </c>
       <c r="O37">
-        <v>909.39399600000002</v>
+        <f t="shared" si="23"/>
+        <v>909.98822098975006</v>
       </c>
       <c r="P37">
-        <v>914.57399511300002</v>
+        <f t="shared" si="23"/>
+        <v>917.41132855425008</v>
       </c>
       <c r="Q37">
-        <v>942.83841705299994</v>
+        <f t="shared" si="23"/>
+        <v>949.99073266999994</v>
       </c>
       <c r="S37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="T37">
+        <f t="shared" ref="T37:Z37" si="24">AVERAGE(T40:T43)</f>
+        <v>117.77808773525004</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="24"/>
+        <v>259.4150921685</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="24"/>
+        <v>6126.5737248002497</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="24"/>
+        <v>111.46875906049999</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="24"/>
+        <v>870.64085799274994</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="24"/>
+        <v>16728.190717983249</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="24"/>
+        <v>9753.9855548100004</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" ref="AC37:AI37" si="25">AVERAGE(AC40:AC43)</f>
+        <v>5.8833917379374991</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="25"/>
+        <v>7.4207723140699997</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="25"/>
+        <v>6053.6734622614495</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="25"/>
+        <v>11.206987023365</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="25"/>
+        <v>792.18774807467503</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="25"/>
+        <v>12006.137218964299</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="25"/>
+        <v>41.569712936850003</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL37">
+        <f t="shared" ref="AL37:AR37" si="26">AVERAGE(AL40:AL43)</f>
+        <v>98.887823701019983</v>
+      </c>
+      <c r="AM37">
+        <f t="shared" si="26"/>
+        <v>240.380842983695</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="26"/>
+        <v>39.427557170375003</v>
+      </c>
+      <c r="AO37">
+        <f t="shared" si="26"/>
+        <v>93.908548176224997</v>
+      </c>
+      <c r="AP37">
+        <f t="shared" si="26"/>
+        <v>48.174330234549998</v>
+      </c>
+      <c r="AQ37">
+        <f t="shared" si="26"/>
+        <v>54.543495059000001</v>
+      </c>
+      <c r="AR37">
+        <f t="shared" si="26"/>
+        <v>1034.3703559022752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ref="B38:H38" si="27">_xlfn.STDEV.P(B40:B43)</f>
+        <v>21.863107613816457</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="27"/>
+        <v>193.75546491220152</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="27"/>
+        <v>6383.3760185485135</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="27"/>
+        <v>11.057839164476862</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="27"/>
+        <v>659.77172602622034</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="27"/>
+        <v>8357.0017550937537</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="27"/>
+        <v>622.09687004841385</v>
+      </c>
+      <c r="J38" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38">
+        <f t="shared" ref="K38:Q38" si="28">_xlfn.STDEV.P(K40:K43)</f>
+        <v>0.11143815192325279</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="28"/>
+        <v>0.22979448905687444</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="28"/>
+        <v>1.0908528333074596</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="28"/>
+        <v>0.16820638644878191</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="28"/>
+        <v>0.86373364660478902</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="28"/>
+        <v>2.9439025499627913</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="28"/>
+        <v>4.3118167796588809</v>
+      </c>
+      <c r="S38" t="s">
+        <v>7</v>
+      </c>
+      <c r="T38">
+        <f t="shared" ref="T38:Z38" si="29">_xlfn.STDEV.P(T40:T43)</f>
+        <v>21.825195783913781</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="29"/>
+        <v>193.64345600977541</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="29"/>
+        <v>6383.8055041672733</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="29"/>
+        <v>11.030484940839022</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="29"/>
+        <v>660.04522505036482</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="29"/>
+        <v>8359.5019360180686</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="29"/>
+        <v>623.78860125519509</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" ref="AC38:AI38" si="30">_xlfn.STDEV.P(AC40:AC43)</f>
+        <v>0.35313093591188971</v>
+      </c>
+      <c r="AD38">
         <f t="shared" si="30"/>
-        <v>111.13463974199999</v>
-      </c>
-      <c r="U37">
+        <v>1.9651214163548025</v>
+      </c>
+      <c r="AE38">
         <f t="shared" si="30"/>
-        <v>94.716400861000011</v>
-      </c>
-      <c r="V37">
+        <v>6391.9680183269165</v>
+      </c>
+      <c r="AF38">
         <f t="shared" si="30"/>
-        <v>8875.0776770159991</v>
-      </c>
-      <c r="W37">
+        <v>1.8928291340794865</v>
+      </c>
+      <c r="AG38">
         <f t="shared" si="30"/>
-        <v>127.29506707499991</v>
-      </c>
-      <c r="X37">
+        <v>657.71312321275275</v>
+      </c>
+      <c r="AH38">
         <f t="shared" si="30"/>
-        <v>1908.8587200599998</v>
-      </c>
-      <c r="Y37">
+        <v>8366.8217040162563</v>
+      </c>
+      <c r="AI38">
         <f t="shared" si="30"/>
-        <v>17347.557379686998</v>
-      </c>
-      <c r="Z37">
-        <f t="shared" si="30"/>
-        <v>10215.940354847</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC37">
-        <v>5.7259418964400002</v>
-      </c>
-      <c r="AD37">
-        <v>5.49935317039</v>
-      </c>
-      <c r="AE37">
-        <v>8804.4597349199994</v>
-      </c>
-      <c r="AF37">
-        <v>10.3173758984</v>
-      </c>
-      <c r="AG37">
-        <v>1829.2179510599999</v>
-      </c>
-      <c r="AH37">
-        <v>12637.018969999999</v>
-      </c>
-      <c r="AI37">
-        <v>39.581485033</v>
-      </c>
-      <c r="AK37" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL37">
-        <v>94.946478843649999</v>
-      </c>
-      <c r="AM37">
-        <v>78.204649925219996</v>
-      </c>
-      <c r="AN37">
-        <v>46.616193056100002</v>
-      </c>
-      <c r="AO37">
-        <v>112.5392789838</v>
-      </c>
-      <c r="AP37">
-        <v>43.515841722499999</v>
-      </c>
-      <c r="AQ37">
-        <v>48.798354387300002</v>
-      </c>
-      <c r="AR37">
-        <v>1486.9329149677001</v>
+        <v>2.79268360747295</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL38">
+        <f t="shared" ref="AL38:AR38" si="31">_xlfn.STDEV.P(AL40:AL43)</f>
+        <v>21.999329583098906</v>
+      </c>
+      <c r="AM38">
+        <f t="shared" si="31"/>
+        <v>195.00233936249393</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="31"/>
+        <v>4.8073559134471058</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="31"/>
+        <v>11.833457020558477</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="31"/>
+        <v>6.4921202615640254</v>
+      </c>
+      <c r="AQ38">
+        <f t="shared" si="31"/>
+        <v>5.9777619372035273</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" si="31"/>
+        <v>609.45872160852252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>1020.21847486</v>
+      </c>
+      <c r="C40">
+        <v>995.70735382999999</v>
+      </c>
+      <c r="D40">
+        <v>1068.9020290399999</v>
+      </c>
+      <c r="E40">
+        <v>1007.61050105</v>
+      </c>
+      <c r="F40">
+        <v>1408.5530149900001</v>
+      </c>
+      <c r="G40">
+        <v>5739.4192831500004</v>
+      </c>
+      <c r="H40">
+        <v>9739.9945700200005</v>
+      </c>
+      <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40">
+        <v>901.53311681699995</v>
+      </c>
+      <c r="L40">
+        <v>903.27882909799996</v>
+      </c>
+      <c r="M40">
+        <v>907.14620685600005</v>
+      </c>
+      <c r="N40">
+        <v>911.01542401300003</v>
+      </c>
+      <c r="O40">
+        <v>908.89405202900002</v>
+      </c>
+      <c r="P40">
+        <v>921.55027008100001</v>
+      </c>
+      <c r="Q40">
+        <v>951.32034492499997</v>
+      </c>
+      <c r="S40" t="s">
+        <v>8</v>
+      </c>
+      <c r="T40">
+        <f t="shared" ref="T40:Z43" si="32">B40-K40</f>
+        <v>118.68535804300006</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="32"/>
+        <v>92.428524732000028</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="32"/>
+        <v>161.75582218399984</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="32"/>
+        <v>96.59507703700001</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="32"/>
+        <v>499.65896296100004</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="32"/>
+        <v>4817.8690130690002</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="32"/>
+        <v>8788.674225095001</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC40">
+        <v>5.4619100093800004</v>
+      </c>
+      <c r="AD40">
+        <v>9.6487638950299992</v>
+      </c>
+      <c r="AE40">
+        <v>95.730875015300001</v>
+      </c>
+      <c r="AF40">
+        <v>12.0980529785</v>
+      </c>
+      <c r="AG40">
+        <v>424.38480997099998</v>
+      </c>
+      <c r="AH40">
+        <v>97.735509157199999</v>
+      </c>
+      <c r="AI40">
+        <v>46.146548986399999</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL40">
+        <v>99.583798885370001</v>
+      </c>
+      <c r="AM40">
+        <v>70.623235940919997</v>
+      </c>
+      <c r="AN40">
+        <v>37.981541872000001</v>
+      </c>
+      <c r="AO40">
+        <v>80.511899948099995</v>
+      </c>
+      <c r="AP40">
+        <v>42.176825761800004</v>
+      </c>
+      <c r="AQ40">
+        <v>52.075365781800002</v>
+      </c>
+      <c r="AR40">
+        <v>82.673387527499997</v>
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>991.73621797600003</v>
+      </c>
+      <c r="C41">
+        <v>1186.92613506</v>
+      </c>
+      <c r="D41">
+        <v>1065.91628098</v>
+      </c>
+      <c r="E41">
+        <v>1024.92551613</v>
+      </c>
+      <c r="F41">
+        <v>1838.1210520300001</v>
+      </c>
+      <c r="G41">
+        <v>29352.296446100001</v>
+      </c>
+      <c r="H41">
+        <v>11334.252119999999</v>
+      </c>
+      <c r="J41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K41">
+        <v>901.45405197100001</v>
+      </c>
+      <c r="L41">
+        <v>903.04278206799995</v>
+      </c>
+      <c r="M41">
+        <v>904.369408131</v>
+      </c>
+      <c r="N41">
+        <v>911.237313986</v>
+      </c>
+      <c r="O41">
+        <v>910.89759898199998</v>
+      </c>
+      <c r="P41">
+        <v>914.68232107200004</v>
+      </c>
+      <c r="Q41">
+        <v>951.40347981499997</v>
+      </c>
+      <c r="S41" t="s">
+        <v>9</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="32"/>
+        <v>90.282166005000022</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="32"/>
+        <v>283.88335299200003</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="32"/>
+        <v>161.54687284900001</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="32"/>
+        <v>113.688202144</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="32"/>
+        <v>927.22345304800012</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="32"/>
+        <v>28437.614125028002</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="32"/>
+        <v>10382.848640184999</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC41">
+        <v>6.4266169071199997</v>
+      </c>
+      <c r="AD41">
+        <v>9.1037890911100003</v>
+      </c>
+      <c r="AE41">
+        <v>67.054330110500004</v>
+      </c>
+      <c r="AF41">
+        <v>13.7307200432</v>
+      </c>
+      <c r="AG41">
+        <v>842.08874511700003</v>
+      </c>
+      <c r="AH41">
+        <v>23736.512354900002</v>
+      </c>
+      <c r="AI41">
+        <v>39.061859846099999</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL41">
+        <v>69.570266008390007</v>
+      </c>
+      <c r="AM41">
+        <v>261.61546802504</v>
+      </c>
+      <c r="AN41">
+        <v>33.2256019115</v>
+      </c>
+      <c r="AO41">
+        <v>88.141054868699996</v>
+      </c>
+      <c r="AP41">
+        <v>58.705394744899998</v>
+      </c>
+      <c r="AQ41">
+        <v>52.729515790900003</v>
+      </c>
+      <c r="AR41">
+        <v>1637.9518008206001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>1052.5203139800001</v>
+      </c>
+      <c r="C42">
+        <v>1470.3024210900001</v>
+      </c>
+      <c r="D42">
+        <v>16212.7773051</v>
+      </c>
+      <c r="E42">
+        <v>1019.05859804</v>
+      </c>
+      <c r="F42">
+        <v>1057.5895328500001</v>
+      </c>
+      <c r="G42">
+        <v>17228.561082100001</v>
+      </c>
+      <c r="H42">
+        <v>10582.879688000001</v>
+      </c>
+      <c r="J42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <v>901.510126829</v>
+      </c>
+      <c r="L42">
+        <v>903.67033100100002</v>
+      </c>
+      <c r="M42">
+        <v>904.86277794800003</v>
+      </c>
+      <c r="N42">
+        <v>910.76190805399995</v>
+      </c>
+      <c r="O42">
+        <v>910.767236948</v>
+      </c>
+      <c r="P42">
+        <v>918.83872795100001</v>
+      </c>
+      <c r="Q42">
+        <v>954.400688887</v>
+      </c>
+      <c r="S42" t="s">
+        <v>10</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="32"/>
+        <v>151.01018715100008</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="32"/>
+        <v>566.63209008900003</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="32"/>
+        <v>15307.914527152001</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="32"/>
+        <v>108.29668998600005</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="32"/>
+        <v>146.82229590200006</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="32"/>
+        <v>16309.722354149</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="32"/>
+        <v>9628.4789991130001</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC42">
+        <v>5.9190981388099999</v>
+      </c>
+      <c r="AD42">
+        <v>5.4311830997500001</v>
+      </c>
+      <c r="AE42">
+        <v>15247.448909000001</v>
+      </c>
+      <c r="AF42">
+        <v>8.68179917336</v>
+      </c>
+      <c r="AG42">
+        <v>73.059486150699996</v>
+      </c>
+      <c r="AH42">
+        <v>11553.282041799999</v>
+      </c>
+      <c r="AI42">
+        <v>41.488957881899999</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL42">
+        <v>131.45075106666999</v>
+      </c>
+      <c r="AM42">
+        <v>551.08001804360003</v>
+      </c>
+      <c r="AN42">
+        <v>39.886891841900002</v>
+      </c>
+      <c r="AO42">
+        <v>94.441958904299995</v>
+      </c>
+      <c r="AP42">
+        <v>48.299258709</v>
+      </c>
+      <c r="AQ42">
+        <v>64.570744275999999</v>
+      </c>
+      <c r="AR42">
+        <v>929.92332029329998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43">
+        <v>1012.38509989</v>
+      </c>
+      <c r="C43">
+        <v>998.16415500599999</v>
+      </c>
+      <c r="D43">
+        <v>9779.8343069599996</v>
+      </c>
+      <c r="E43">
+        <v>1038.3013410599999</v>
+      </c>
+      <c r="F43">
+        <v>2818.2527160599998</v>
+      </c>
+      <c r="G43">
+        <v>18262.131374799999</v>
+      </c>
+      <c r="H43">
+        <v>11158.778771900001</v>
+      </c>
+      <c r="J43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43">
+        <v>901.250460148</v>
+      </c>
+      <c r="L43">
+        <v>903.44775414499998</v>
+      </c>
+      <c r="M43">
+        <v>904.756629944</v>
+      </c>
+      <c r="N43">
+        <v>911.00627398500001</v>
+      </c>
+      <c r="O43">
+        <v>909.39399600000002</v>
+      </c>
+      <c r="P43">
+        <v>914.57399511300002</v>
+      </c>
+      <c r="Q43">
+        <v>942.83841705299994</v>
+      </c>
+      <c r="S43" t="s">
+        <v>11</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="32"/>
+        <v>111.13463974199999</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="32"/>
+        <v>94.716400861000011</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="32"/>
+        <v>8875.0776770159991</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="32"/>
+        <v>127.29506707499991</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="32"/>
+        <v>1908.8587200599998</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="32"/>
+        <v>17347.557379686998</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="32"/>
+        <v>10215.940354847</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC43">
+        <v>5.7259418964400002</v>
+      </c>
+      <c r="AD43">
+        <v>5.49935317039</v>
+      </c>
+      <c r="AE43">
+        <v>8804.4597349199994</v>
+      </c>
+      <c r="AF43">
+        <v>10.3173758984</v>
+      </c>
+      <c r="AG43">
+        <v>1829.2179510599999</v>
+      </c>
+      <c r="AH43">
+        <v>12637.018969999999</v>
+      </c>
+      <c r="AI43">
+        <v>39.581485033</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL43">
+        <v>94.946478843649999</v>
+      </c>
+      <c r="AM43">
+        <v>78.204649925219996</v>
+      </c>
+      <c r="AN43">
+        <v>46.616193056100002</v>
+      </c>
+      <c r="AO43">
+        <v>112.5392789838</v>
+      </c>
+      <c r="AP43">
+        <v>43.515841722499999</v>
+      </c>
+      <c r="AQ43">
+        <v>48.798354387300002</v>
+      </c>
+      <c r="AR43">
+        <v>1486.9329149677001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8258,8 +8595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P70:S71"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="AE80" sqref="AE80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS77" sqref="AS77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8287,13 +8624,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -8351,10 +8693,10 @@
         <v>21.863107613816499</v>
       </c>
       <c r="D6">
-        <v>1343.6227599399999</v>
+        <v>1525.8971184787499</v>
       </c>
       <c r="E6">
-        <v>389.95321554157999</v>
+        <v>330.55075412857184</v>
       </c>
       <c r="F6">
         <v>1939.5044540174999</v>
@@ -8377,10 +8719,10 @@
         <v>193.755464912202</v>
       </c>
       <c r="D7">
-        <v>1355.4074729675001</v>
+        <v>1195.15302783125</v>
       </c>
       <c r="E7">
-        <v>2.1150456385541001</v>
+        <v>160.49379901294051</v>
       </c>
       <c r="F7">
         <v>1922.3329895750001</v>
@@ -8403,10 +8745,10 @@
         <v>11.057839164476899</v>
       </c>
       <c r="D8">
-        <v>1487.1671472200001</v>
+        <v>1539.4759002325</v>
       </c>
       <c r="E8">
-        <v>387.64944318789901</v>
+        <v>282.44061723090124</v>
       </c>
       <c r="F8">
         <v>1971.5520235874999</v>
@@ -8429,10 +8771,10 @@
         <v>622.09687004841396</v>
       </c>
       <c r="D9">
-        <v>2331.0594869249999</v>
+        <v>3052.8215979325005</v>
       </c>
       <c r="E9">
-        <v>115.494131234116</v>
+        <v>734.45939887387738</v>
       </c>
       <c r="F9">
         <v>2835.0577372325001</v>
@@ -8494,10 +8836,10 @@
         <v>21.825195783913799</v>
       </c>
       <c r="D16">
-        <v>127.54590612749996</v>
+        <v>128.47338133962498</v>
       </c>
       <c r="E16">
-        <v>5.2901632702800718</v>
+        <v>7.0244094563688133</v>
       </c>
       <c r="F16">
         <v>134.39133900499999</v>
@@ -8517,10 +8859,10 @@
         <v>193.64345600977501</v>
       </c>
       <c r="D17">
-        <v>144.02130383000008</v>
+        <v>131.04659050475004</v>
       </c>
       <c r="E17">
-        <v>16.931162871998762</v>
+        <v>19.305037162582359</v>
       </c>
       <c r="F17">
         <v>117.68353009499999</v>
@@ -8540,10 +8882,10 @@
         <v>11.030484940839001</v>
       </c>
       <c r="D18">
-        <v>222.60707020750004</v>
+        <v>176.592414587375</v>
       </c>
       <c r="E18">
-        <v>43.021244097630778</v>
+        <v>55.598549503909751</v>
       </c>
       <c r="F18">
         <v>140.19159406</v>
@@ -8563,16 +8905,105 @@
         <v>623.78860125519498</v>
       </c>
       <c r="D19">
-        <v>542.69585400750009</v>
+        <v>363.74241572375007</v>
       </c>
       <c r="E19">
-        <v>123.55531007138792</v>
+        <v>199.55844957340665</v>
       </c>
       <c r="F19">
         <v>209.6199097075</v>
       </c>
       <c r="G19">
         <v>5.41536815417673</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <f>AVERAGE(B16,D16,F16)</f>
+        <v>126.88093602662498</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>5424.432282947083</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:B28" si="0">AVERAGE(B17,D17,F17)</f>
+        <v>169.38173758941667</v>
+      </c>
+      <c r="C26">
+        <v>16048.522537510391</v>
+      </c>
+      <c r="D26">
+        <v>70575.255633700814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>256</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>142.75092256929167</v>
+      </c>
+      <c r="C27">
+        <v>22703.596674211436</v>
+      </c>
+      <c r="D27">
+        <v>41946.515345922933</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2048</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>3442.4492934137502</v>
+      </c>
+      <c r="C28">
+        <v>37794.757197262959</v>
+      </c>
+      <c r="D28">
+        <v>37223.38461279581</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pes for 2 and 4 resources
</commit_message>
<xml_diff>
--- a/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
+++ b/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/AIMES_Experiments/Summary Files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="45" windowWidth="28005" windowHeight="16440" tabRatio="462" activeTab="1"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="28000" windowHeight="16440" tabRatio="462" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Timings_AIMES" sheetId="1" r:id="rId1"/>
-    <sheet name="Plots" sheetId="2" r:id="rId2"/>
-    <sheet name="Plot Data" sheetId="3" r:id="rId3"/>
-    <sheet name="AS paper plots" sheetId="4" r:id="rId4"/>
+    <sheet name="Pes" sheetId="5" r:id="rId2"/>
+    <sheet name="Plots" sheetId="2" r:id="rId3"/>
+    <sheet name="Plot Data" sheetId="3" r:id="rId4"/>
+    <sheet name="AS paper plots" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
   <si>
     <t>TTC_AIMES_SWIFT_1_v2</t>
   </si>
@@ -155,6 +164,42 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>SDEV</t>
+  </si>
+  <si>
+    <t>run 1</t>
+  </si>
+  <si>
+    <t>run 2</t>
+  </si>
+  <si>
+    <t>run 3</t>
+  </si>
+  <si>
+    <t>run 4</t>
+  </si>
+  <si>
+    <t>run 5</t>
+  </si>
+  <si>
+    <t>run 6</t>
+  </si>
+  <si>
+    <t>run 7</t>
+  </si>
+  <si>
+    <t>run 8</t>
+  </si>
+  <si>
+    <t>TTCi</t>
+  </si>
+  <si>
+    <t>TTCm, Gordon and Stampede</t>
+  </si>
+  <si>
+    <t>TTCm, Gordon, Stampede, Comet, SuperMIC</t>
+  </si>
 </sst>
 </file>
 
@@ -182,15 +227,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -198,17 +249,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,16 +442,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.863107613816499</c:v>
+                    <c:v>21.8631076138165</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>193.755464912202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.057839164476899</c:v>
+                    <c:v>11.0578391644769</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>622.09687004841396</c:v>
+                    <c:v>622.096870048414</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -377,16 +463,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.863107613816499</c:v>
+                    <c:v>21.8631076138165</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>193.755464912202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.057839164476899</c:v>
+                    <c:v>11.0578391644769</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>622.09687004841396</c:v>
+                    <c:v>622.096870048414</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -399,16 +485,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,7 +509,7 @@
                   <c:v>1019.2150266765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162.7750162464999</c:v>
+                  <c:v>1162.7750162465</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1022.47398907</c:v>
@@ -454,16 +540,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -475,16 +561,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -497,7 +583,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1525.8971184787499</c:v>
+                  <c:v>1525.89711847875</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1195.15302783125</c:v>
@@ -506,7 +592,7 @@
                   <c:v>1539.4759002325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3052.8215979325005</c:v>
+                  <c:v>3052.8215979325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,16 +621,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -556,16 +642,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -578,16 +664,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1939.5044540174999</c:v>
+                  <c:v>1939.5044540175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1922.3329895750001</c:v>
+                  <c:v>1922.332989575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1971.5520235874999</c:v>
+                  <c:v>1971.5520235875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2835.0577372325001</c:v>
+                  <c:v>2835.0577372325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,16 +702,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,11 +728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238288256"/>
-        <c:axId val="238560768"/>
+        <c:axId val="-2082219072"/>
+        <c:axId val="-2090035408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238288256"/>
+        <c:axId val="-2082219072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238560768"/>
+        <c:crossAx val="-2090035408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -664,10 +750,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238560768"/>
+        <c:axId val="-2090035408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -676,10 +762,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238288256"/>
+        <c:crossAx val="-2082219072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -819,6 +905,37 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -868,13 +985,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -889,13 +1006,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -924,16 +1041,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,10 +1062,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>134.39133900499999</c:v>
+                  <c:v>134.391339005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.68353009499999</c:v>
+                  <c:v>117.683530095</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>140.19159406</c:v>
@@ -971,11 +1088,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238367872"/>
-        <c:axId val="238369792"/>
+        <c:axId val="-2102436464"/>
+        <c:axId val="-2043032064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238367872"/>
+        <c:axId val="-2102436464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,6 +1137,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1055,7 +1189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238369792"/>
+        <c:crossAx val="-2043032064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1063,11 +1197,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238369792"/>
+        <c:axId val="-2043032064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
-          <c:min val="0"/>
+          <c:max val="60000.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1143,6 +1277,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1172,7 +1323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238367872"/>
+        <c:crossAx val="-2102436464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1306,16 +1457,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.825195783913799</c:v>
+                    <c:v>21.8251957839138</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>193.64345600977501</c:v>
+                    <c:v>193.643456009775</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.030484940839001</c:v>
+                    <c:v>11.030484940839</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>623.78860125519498</c:v>
+                    <c:v>623.788601255195</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1327,16 +1478,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.825195783913799</c:v>
+                    <c:v>21.8251957839138</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>193.64345600977501</c:v>
+                    <c:v>193.643456009775</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.030484940839001</c:v>
+                    <c:v>11.030484940839</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>623.78860125519498</c:v>
+                    <c:v>623.788601255195</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1349,16 +1500,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1376,10 +1527,10 @@
                   <c:v>259.4150921685</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>111.46875906050001</c:v>
+                  <c:v>111.4687590605</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9753.9855548100004</c:v>
+                  <c:v>9753.98555481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,16 +1555,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>7.0244094563688133</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.305037162582359</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.598549503909751</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>199.55844957340665</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1425,16 +1576,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>7.0244094563688133</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.305037162582359</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.598549503909751</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>199.55844957340665</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1447,16 +1598,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1468,16 +1619,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128.47338133962498</c:v>
+                  <c:v>128.473381339625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131.04659050475004</c:v>
+                  <c:v>131.04659050475</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>176.592414587375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>363.74241572375007</c:v>
+                  <c:v>363.74241572375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,13 +1657,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -1527,13 +1678,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -1549,16 +1700,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1570,10 +1721,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>134.39133900499999</c:v>
+                  <c:v>134.391339005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.68353009499999</c:v>
+                  <c:v>117.683530095</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>140.19159406</c:v>
@@ -1596,11 +1747,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238604672"/>
-        <c:axId val="238606208"/>
+        <c:axId val="-2042734672"/>
+        <c:axId val="-2043327808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238604672"/>
+        <c:axId val="-2042734672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238606208"/>
+        <c:crossAx val="-2043327808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1618,10 +1769,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238606208"/>
+        <c:axId val="-2043327808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1630,10 +1781,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238604672"/>
+        <c:crossAx val="-2042734672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1730,16 +1881,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.863107613816499</c:v>
+                    <c:v>21.8631076138165</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>193.755464912202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.057839164476899</c:v>
+                    <c:v>11.0578391644769</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>622.09687004841396</c:v>
+                    <c:v>622.096870048414</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1751,16 +1902,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.863107613816499</c:v>
+                    <c:v>21.8631076138165</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>193.755464912202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.057839164476899</c:v>
+                    <c:v>11.0578391644769</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>622.09687004841396</c:v>
+                    <c:v>622.096870048414</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1773,16 +1924,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1797,7 +1948,7 @@
                   <c:v>1019.2150266765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162.7750162464999</c:v>
+                  <c:v>1162.7750162465</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1022.47398907</c:v>
@@ -1832,16 +1983,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1858,11 +2009,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="238910080"/>
-        <c:axId val="238920448"/>
+        <c:axId val="-2087339120"/>
+        <c:axId val="-2043103280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="238910080"/>
+        <c:axId val="-2087339120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,7 +2023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238920448"/>
+        <c:crossAx val="-2043103280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1880,10 +2031,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238920448"/>
+        <c:axId val="-2043103280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1892,10 +2043,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238910080"/>
+        <c:crossAx val="-2087339120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1988,16 +2139,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2009,16 +2160,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>330.55075412857184</c:v>
+                    <c:v>330.5507541285718</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>160.49379901294051</c:v>
+                    <c:v>160.4937990129405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>282.44061723090124</c:v>
+                    <c:v>282.4406172309012</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>734.45939887387738</c:v>
+                    <c:v>734.4593988738773</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2031,16 +2182,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,7 +2203,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1525.8971184787499</c:v>
+                  <c:v>1525.89711847875</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1195.15302783125</c:v>
@@ -2061,7 +2212,7 @@
                   <c:v>1539.4759002325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3052.8215979325005</c:v>
+                  <c:v>3052.8215979325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,16 +2241,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,16 +2262,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2137,11 +2288,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239012864"/>
-        <c:axId val="239019136"/>
+        <c:axId val="-2097872752"/>
+        <c:axId val="-2098061168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239012864"/>
+        <c:axId val="-2097872752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2151,7 +2302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239019136"/>
+        <c:crossAx val="-2098061168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2159,10 +2310,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239019136"/>
+        <c:axId val="-2098061168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2171,10 +2322,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239012864"/>
+        <c:crossAx val="-2097872752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2274,13 +2425,13 @@
                     <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>5.25514853659808</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>625.412181601585</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2295,13 +2446,13 @@
                     <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>5.25514853659808</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>625.412181601585</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2314,16 +2465,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,16 +2486,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1939.5044540174999</c:v>
+                  <c:v>1939.5044540175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1922.3329895750001</c:v>
+                  <c:v>1922.332989575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1971.5520235874999</c:v>
+                  <c:v>1971.5520235875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2835.0577372325001</c:v>
+                  <c:v>2835.0577372325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2373,16 +2524,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2394,16 +2545,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2420,11 +2571,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239053056"/>
-        <c:axId val="239055232"/>
+        <c:axId val="-2087282336"/>
+        <c:axId val="-2086633952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239053056"/>
+        <c:axId val="-2087282336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,7 +2585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239055232"/>
+        <c:crossAx val="-2086633952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2442,10 +2593,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239055232"/>
+        <c:axId val="-2086633952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2454,10 +2605,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239053056"/>
+        <c:crossAx val="-2087282336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2555,16 +2706,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.825195783913799</c:v>
+                    <c:v>21.8251957839138</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>193.64345600977501</c:v>
+                    <c:v>193.643456009775</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.030484940839001</c:v>
+                    <c:v>11.030484940839</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>623.78860125519498</c:v>
+                    <c:v>623.788601255195</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2576,16 +2727,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>21.825195783913799</c:v>
+                    <c:v>21.8251957839138</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>193.64345600977501</c:v>
+                    <c:v>193.643456009775</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.030484940839001</c:v>
+                    <c:v>11.030484940839</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>623.78860125519498</c:v>
+                    <c:v>623.788601255195</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2598,16 +2749,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2625,10 +2776,10 @@
                   <c:v>259.4150921685</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>111.46875906050001</c:v>
+                  <c:v>111.4687590605</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9753.9855548100004</c:v>
+                  <c:v>9753.98555481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2645,11 +2796,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239062016"/>
-        <c:axId val="239067904"/>
+        <c:axId val="-2086974224"/>
+        <c:axId val="-2043316816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239062016"/>
+        <c:axId val="-2086974224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +2810,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239067904"/>
+        <c:crossAx val="-2043316816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2667,10 +2818,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239067904"/>
+        <c:axId val="-2043316816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2679,10 +2830,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239062016"/>
+        <c:crossAx val="-2086974224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2776,16 +2927,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>7.0244094563688133</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.305037162582359</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.598549503909751</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>199.55844957340665</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2797,16 +2948,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>7.0244094563688133</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.305037162582359</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.598549503909751</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>199.55844957340665</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2819,16 +2970,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2840,16 +2991,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>128.47338133962498</c:v>
+                  <c:v>128.473381339625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131.04659050475004</c:v>
+                  <c:v>131.04659050475</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>176.592414587375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>363.74241572375007</c:v>
+                  <c:v>363.74241572375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2866,11 +3017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239125632"/>
-        <c:axId val="239127168"/>
+        <c:axId val="-2087093712"/>
+        <c:axId val="-2086137904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239125632"/>
+        <c:axId val="-2087093712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +3031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239127168"/>
+        <c:crossAx val="-2086137904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2888,10 +3039,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239127168"/>
+        <c:axId val="-2086137904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2900,10 +3051,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239125632"/>
+        <c:crossAx val="-2087093712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3000,13 +3151,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -3021,13 +3172,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.092325359198099</c:v>
+                    <c:v>22.0923253591981</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8232656449817197</c:v>
+                    <c:v>4.82326564498172</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.2386943213578503</c:v>
+                    <c:v>6.23869432135785</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.41536815417673</c:v>
@@ -3043,16 +3194,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3064,10 +3215,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>134.39133900499999</c:v>
+                  <c:v>134.391339005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.68353009499999</c:v>
+                  <c:v>117.683530095</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>140.19159406</c:v>
@@ -3090,11 +3241,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239139840"/>
-        <c:axId val="239158016"/>
+        <c:axId val="-2043360160"/>
+        <c:axId val="-2043357360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239139840"/>
+        <c:axId val="-2043360160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,7 +3255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239158016"/>
+        <c:crossAx val="-2043357360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3112,10 +3263,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239158016"/>
+        <c:axId val="-2043357360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
+          <c:max val="60000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3124,10 +3275,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239139840"/>
+        <c:crossAx val="-2043360160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10000"/>
+        <c:majorUnit val="10000.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3229,6 +3380,40 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3281,13 +3466,13 @@
                     <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>5.25514853659808</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>625.412181601585</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3302,13 +3487,13 @@
                     <c:v>21.3459437562951</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2551485365980799</c:v>
+                    <c:v>5.25514853659808</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.6882619440157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>625.41218160158496</c:v>
+                    <c:v>625.412181601585</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3334,16 +3519,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3355,16 +3540,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1939.5044540174999</c:v>
+                  <c:v>1939.5044540175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1922.3329895750001</c:v>
+                  <c:v>1922.332989575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1971.5520235874999</c:v>
+                  <c:v>1971.5520235875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2835.0577372325001</c:v>
+                  <c:v>2835.0577372325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3408,16 +3593,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3429,16 +3614,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3455,11 +3640,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239228032"/>
-        <c:axId val="239230336"/>
+        <c:axId val="-2043303680"/>
+        <c:axId val="-2043514640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239228032"/>
+        <c:axId val="-2043303680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,6 +3689,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3539,7 +3741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239230336"/>
+        <c:crossAx val="-2043514640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3547,11 +3749,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239230336"/>
+        <c:axId val="-2043514640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000"/>
-          <c:min val="0"/>
+          <c:max val="60000.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3627,6 +3829,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3656,7 +3875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239228032"/>
+        <c:crossAx val="-2043303680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3726,7 +3945,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId1"/>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -5454,7 +5673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5465,12 +5684,12 @@
   <dimension ref="A1:AR47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z18" activeCellId="2" sqref="T18:U19 W18:W19 Z18:Z19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5502,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -5624,7 +5843,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5781,7 +6000,7 @@
         <v>1166.6673192692499</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5938,7 +6157,7 @@
         <v>705.49640013527494</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5949,7 +6168,7 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -6078,7 +6297,7 @@
         <v>795.76181566699995</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6207,7 +6426,7 @@
         <v>750.45791912100003</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6336,7 +6555,7 @@
         <v>2387.9700789499998</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -6465,7 +6684,7 @@
         <v>732.47946333899995</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -6494,7 +6713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -6616,7 +6835,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -6761,7 +6980,7 @@
         <v>2409.5385053177502</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -6906,7 +7125,7 @@
         <v>100.88058932003152</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -7026,7 +7245,7 @@
         <v>2254.0199455050001</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -7146,7 +7365,7 @@
         <v>2529.0927404200002</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -7266,7 +7485,7 @@
         <v>2399.3993296610001</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7386,7 +7605,7 @@
         <v>2455.6420056850002</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -7437,7 +7656,7 @@
         <v>160.42066788000011</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -7488,7 +7707,7 @@
         <v>176.32802318999984</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -7539,7 +7758,7 @@
         <v>209.14063191000014</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -7590,12 +7809,12 @@
         <v>193.26658678000013</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.15">
       <c r="J30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -7624,7 +7843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -7746,7 +7965,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -7903,7 +8122,7 @@
         <v>1034.3703559022752</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -8060,7 +8279,7 @@
         <v>609.45872160852252</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -8189,7 +8408,7 @@
         <v>82.673387527499997</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -8318,7 +8537,7 @@
         <v>1637.9518008206001</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -8447,7 +8666,7 @@
         <v>929.92332029329998</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -8576,7 +8795,7 @@
         <v>1486.9329149677001</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -8593,20 +8812,661 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9">
+        <v>256</v>
+      </c>
+      <c r="E2" s="9">
+        <v>2048</v>
+      </c>
+      <c r="G2" s="4">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4">
+        <v>256</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2048</v>
+      </c>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9">
+        <v>8</v>
+      </c>
+      <c r="N2" s="9">
+        <v>32</v>
+      </c>
+      <c r="O2" s="9">
+        <v>256</v>
+      </c>
+      <c r="P2" s="9">
+        <v>2048</v>
+      </c>
+      <c r="R2" s="4">
+        <v>8</v>
+      </c>
+      <c r="S2" s="4">
+        <v>32</v>
+      </c>
+      <c r="T2" s="4">
+        <v>256</v>
+      </c>
+      <c r="U2" s="4">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <f>AVERAGE(B5:B12)</f>
+        <v>61.841558147279173</v>
+      </c>
+      <c r="C3" s="6">
+        <f>AVERAGE(C5:C12)</f>
+        <v>76.685731073253208</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:E3" si="0">AVERAGE(D5:D12)</f>
+        <v>60.518231391865697</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>31.317576403829655</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6">
+        <f>AVERAGE(M5:M12)</f>
+        <v>46.409181084802611</v>
+      </c>
+      <c r="N3" s="6">
+        <f>AVERAGE(N5:N12)</f>
+        <v>46.818461236666039</v>
+      </c>
+      <c r="O3" s="6">
+        <f t="shared" ref="O3:P3" si="1">AVERAGE(O5:O12)</f>
+        <v>45.654304727452079</v>
+      </c>
+      <c r="P3" s="6">
+        <f t="shared" si="1"/>
+        <v>33.026460757769961</v>
+      </c>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="7">
+        <f>_xlfn.STDEV.S(B5:B12)</f>
+        <v>14.377193500625335</v>
+      </c>
+      <c r="C4" s="7">
+        <f>_xlfn.STDEV.S(C5:C12)</f>
+        <v>10.999453965314661</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" ref="D4:E4" si="2">_xlfn.STDEV.S(D5:D12)</f>
+        <v>12.305393956240616</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="2"/>
+        <v>8.1919046267088227</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="7">
+        <f>_xlfn.STDEV.S(M5:M12)</f>
+        <v>0.58496667889487797</v>
+      </c>
+      <c r="N4" s="7">
+        <f>_xlfn.STDEV.S(N5:N12)</f>
+        <v>0.14777925926362356</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" ref="O4" si="3">_xlfn.STDEV.S(O5:O12)</f>
+        <v>0.54905565173586512</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" ref="P4" si="4">_xlfn.STDEV.S(P5:P12)</f>
+        <v>6.7057964381049793</v>
+      </c>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6">
+        <f>(G5/Timings_AIMES!B21)*100</f>
+        <v>66.693946069526532</v>
+      </c>
+      <c r="C5" s="6">
+        <f>(H5/Timings_AIMES!C21)*100</f>
+        <v>66.507683490931043</v>
+      </c>
+      <c r="D5" s="6">
+        <f>(I5/Timings_AIMES!E21)*100</f>
+        <v>58.367357950824491</v>
+      </c>
+      <c r="E5" s="6">
+        <f>(J5/Timings_AIMES!H21)*100</f>
+        <v>34.771844060017067</v>
+      </c>
+      <c r="G5" s="5">
+        <v>900</v>
+      </c>
+      <c r="H5" s="5">
+        <v>900</v>
+      </c>
+      <c r="I5" s="5">
+        <v>900</v>
+      </c>
+      <c r="J5" s="5">
+        <v>900</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <f>(R5/Timings_AIMES!B8)*100</f>
+        <v>46.62041026262758</v>
+      </c>
+      <c r="N5" s="6">
+        <f>(S5/Timings_AIMES!C8)*100</f>
+        <v>46.910459395875911</v>
+      </c>
+      <c r="O5" s="6">
+        <f>(T5/Timings_AIMES!E8)*100</f>
+        <v>44.884591277688934</v>
+      </c>
+      <c r="P5" s="6">
+        <f>(U5/Timings_AIMES!H8)*100</f>
+        <v>36.243343067307421</v>
+      </c>
+      <c r="R5" s="5">
+        <v>900</v>
+      </c>
+      <c r="S5" s="5">
+        <v>900</v>
+      </c>
+      <c r="T5" s="5">
+        <v>900</v>
+      </c>
+      <c r="U5" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="6">
+        <f>(G6/Timings_AIMES!B22)*100</f>
+        <v>67.185700995393731</v>
+      </c>
+      <c r="C6" s="6">
+        <f>(H6/Timings_AIMES!C22)*100</f>
+        <v>67.111610386239732</v>
+      </c>
+      <c r="D6" s="6">
+        <f>(I6/Timings_AIMES!E22)*100</f>
+        <v>63.321554075126407</v>
+      </c>
+      <c r="E6" s="6">
+        <f>(J6/Timings_AIMES!H22)*100</f>
+        <v>39.245140548680581</v>
+      </c>
+      <c r="G6" s="5">
+        <v>900</v>
+      </c>
+      <c r="H6" s="5">
+        <v>900</v>
+      </c>
+      <c r="I6" s="5">
+        <v>900</v>
+      </c>
+      <c r="J6" s="5">
+        <v>900</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="6">
+        <f>(R6/Timings_AIMES!B9)*100</f>
+        <v>45.585609815962592</v>
+      </c>
+      <c r="N6" s="6">
+        <f>(S6/Timings_AIMES!C9)*100</f>
+        <v>46.9734647730441</v>
+      </c>
+      <c r="O6" s="6">
+        <f>(T6/Timings_AIMES!E9)*100</f>
+        <v>45.730806522660714</v>
+      </c>
+      <c r="P6" s="6">
+        <f>(U6/Timings_AIMES!H9)*100</f>
+        <v>36.343620618692334</v>
+      </c>
+      <c r="R6" s="5">
+        <v>900</v>
+      </c>
+      <c r="S6" s="5">
+        <v>900</v>
+      </c>
+      <c r="T6" s="5">
+        <v>900</v>
+      </c>
+      <c r="U6" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6">
+        <f>(G7/Timings_AIMES!B23)*100</f>
+        <v>67.154383342188936</v>
+      </c>
+      <c r="C7" s="6">
+        <f>(H7/Timings_AIMES!C23)*100</f>
+        <v>65.462821101089062</v>
+      </c>
+      <c r="D7" s="6">
+        <f>(I7/Timings_AIMES!E23)*100</f>
+        <v>57.871720709776028</v>
+      </c>
+      <c r="E7" s="6">
+        <f>(J7/Timings_AIMES!H23)*100</f>
+        <v>39.835406349457365</v>
+      </c>
+      <c r="G7" s="5">
+        <v>900</v>
+      </c>
+      <c r="H7" s="5">
+        <v>900</v>
+      </c>
+      <c r="I7" s="5">
+        <v>900</v>
+      </c>
+      <c r="J7" s="5">
+        <v>900</v>
+      </c>
+      <c r="L7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="6">
+        <f>(R7/Timings_AIMES!B10)*100</f>
+        <v>46.474323887551947</v>
+      </c>
+      <c r="N7" s="6">
+        <f>(S7/Timings_AIMES!C10)*100</f>
+        <v>46.730467092507851</v>
+      </c>
+      <c r="O7" s="6">
+        <f>(T7/Timings_AIMES!E10)*100</f>
+        <v>46.182299374241126</v>
+      </c>
+      <c r="P7" s="6">
+        <f>(U7/Timings_AIMES!H10)*100</f>
+        <v>22.969580221531459</v>
+      </c>
+      <c r="R7" s="5">
+        <v>900</v>
+      </c>
+      <c r="S7" s="5">
+        <v>900</v>
+      </c>
+      <c r="T7" s="5">
+        <v>900</v>
+      </c>
+      <c r="U7" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6">
+        <f>(G8/Timings_AIMES!B24)*100</f>
+        <v>66.900719828089251</v>
+      </c>
+      <c r="C8" s="6">
+        <f>(H8/Timings_AIMES!C24)*100</f>
+        <v>66.542110436826476</v>
+      </c>
+      <c r="D8" s="6">
+        <f>(I8/Timings_AIMES!E24)*100</f>
+        <v>62.926935399951276</v>
+      </c>
+      <c r="E8" s="6">
+        <f>(J8/Timings_AIMES!H24)*100</f>
+        <v>41.220819443716138</v>
+      </c>
+      <c r="G8" s="5">
+        <v>900</v>
+      </c>
+      <c r="H8" s="5">
+        <v>900</v>
+      </c>
+      <c r="I8" s="5">
+        <v>900</v>
+      </c>
+      <c r="J8" s="5">
+        <v>900</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="6">
+        <f>(R8/Timings_AIMES!B11)*100</f>
+        <v>46.95638037306832</v>
+      </c>
+      <c r="N8" s="6">
+        <f>(S8/Timings_AIMES!C11)*100</f>
+        <v>46.659453685236322</v>
+      </c>
+      <c r="O8" s="6">
+        <f>(T8/Timings_AIMES!E11)*100</f>
+        <v>45.819521735217535</v>
+      </c>
+      <c r="P8" s="6">
+        <f>(U8/Timings_AIMES!H11)*100</f>
+        <v>36.549299123548629</v>
+      </c>
+      <c r="R8" s="5">
+        <v>900</v>
+      </c>
+      <c r="S8" s="5">
+        <v>900</v>
+      </c>
+      <c r="T8" s="5">
+        <v>900</v>
+      </c>
+      <c r="U8" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6">
+        <f>(G9/Timings_AIMES!B25)*100</f>
+        <v>46.845699378199988</v>
+      </c>
+      <c r="C9" s="6">
+        <f>(H9/Timings_AIMES!C25)*100</f>
+        <v>87.066298383023408</v>
+      </c>
+      <c r="D9" s="6">
+        <f>(I9/Timings_AIMES!E25)*100</f>
+        <v>84.610765831843665</v>
+      </c>
+      <c r="E9" s="6">
+        <f>(J9/Timings_AIMES!H25)*100</f>
+        <v>25.177472119161266</v>
+      </c>
+      <c r="G9" s="5">
+        <v>900</v>
+      </c>
+      <c r="H9" s="5">
+        <v>900</v>
+      </c>
+      <c r="I9" s="5">
+        <v>900</v>
+      </c>
+      <c r="J9" s="5">
+        <v>900</v>
+      </c>
+      <c r="L9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="R9" s="5">
+        <v>900</v>
+      </c>
+      <c r="S9" s="5">
+        <v>900</v>
+      </c>
+      <c r="T9" s="5">
+        <v>900</v>
+      </c>
+      <c r="U9" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6">
+        <f>(G10/Timings_AIMES!B26)*100</f>
+        <v>46.463587320050131</v>
+      </c>
+      <c r="C10" s="6">
+        <f>(H10/Timings_AIMES!C26)*100</f>
+        <v>86.668518413904906</v>
+      </c>
+      <c r="D10" s="6">
+        <f>(I10/Timings_AIMES!E26)*100</f>
+        <v>45.670166120303783</v>
+      </c>
+      <c r="E10" s="6">
+        <f>(J10/Timings_AIMES!H26)*100</f>
+        <v>23.418596825647199</v>
+      </c>
+      <c r="G10" s="5">
+        <v>900</v>
+      </c>
+      <c r="H10" s="5">
+        <v>900</v>
+      </c>
+      <c r="I10" s="5">
+        <v>900</v>
+      </c>
+      <c r="J10" s="5">
+        <v>900</v>
+      </c>
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="R10" s="5">
+        <v>900</v>
+      </c>
+      <c r="S10" s="5">
+        <v>900</v>
+      </c>
+      <c r="T10" s="5">
+        <v>900</v>
+      </c>
+      <c r="U10" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="6">
+        <f>(G11/Timings_AIMES!B27)*100</f>
+        <v>87.135011712013551</v>
+      </c>
+      <c r="C11" s="6">
+        <f>(H11/Timings_AIMES!C27)*100</f>
+        <v>87.128008165694553</v>
+      </c>
+      <c r="D11" s="6">
+        <f>(I11/Timings_AIMES!E27)*100</f>
+        <v>65.360899070715405</v>
+      </c>
+      <c r="E11" s="6">
+        <f>(J11/Timings_AIMES!H27)*100</f>
+        <v>23.4088533493886</v>
+      </c>
+      <c r="G11" s="5">
+        <v>900</v>
+      </c>
+      <c r="H11" s="5">
+        <v>900</v>
+      </c>
+      <c r="I11" s="5">
+        <v>900</v>
+      </c>
+      <c r="J11" s="5">
+        <v>900</v>
+      </c>
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="R11" s="5">
+        <v>900</v>
+      </c>
+      <c r="S11" s="5">
+        <v>900</v>
+      </c>
+      <c r="T11" s="5">
+        <v>900</v>
+      </c>
+      <c r="U11" s="5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6">
+        <f>(G12/Timings_AIMES!B28)*100</f>
+        <v>46.353416532771227</v>
+      </c>
+      <c r="C12" s="6">
+        <f>(H12/Timings_AIMES!C28)*100</f>
+        <v>86.998798208316401</v>
+      </c>
+      <c r="D12" s="6">
+        <f>(I12/Timings_AIMES!E28)*100</f>
+        <v>46.016451976384531</v>
+      </c>
+      <c r="E12" s="6">
+        <f>(J12/Timings_AIMES!H28)*100</f>
+        <v>23.462478534568973</v>
+      </c>
+      <c r="G12" s="5">
+        <v>900</v>
+      </c>
+      <c r="H12" s="5">
+        <v>900</v>
+      </c>
+      <c r="I12" s="5">
+        <v>900</v>
+      </c>
+      <c r="J12" s="5">
+        <v>900</v>
+      </c>
+      <c r="L12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="R12" s="5">
+        <v>900</v>
+      </c>
+      <c r="S12" s="5">
+        <v>900</v>
+      </c>
+      <c r="T12" s="5">
+        <v>900</v>
+      </c>
+      <c r="U12" s="5">
+        <v>900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P70:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="I15" workbookViewId="0">
       <selection activeCell="AS77" sqref="AS77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="70" spans="16:19" x14ac:dyDescent="0.2">
+    <row r="70" spans="16:19" x14ac:dyDescent="0.15">
       <c r="P70" s="1"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
     </row>
-    <row r="71" spans="16:19" x14ac:dyDescent="0.2">
+    <row r="71" spans="16:19" x14ac:dyDescent="0.15">
       <c r="P71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
@@ -8622,7 +9482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H32"/>
   <sheetViews>
@@ -8630,19 +9490,19 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -8656,7 +9516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -8682,7 +9542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>8</v>
       </c>
@@ -8708,7 +9568,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>32</v>
       </c>
@@ -8734,7 +9594,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>256</v>
       </c>
@@ -8760,7 +9620,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2048</v>
       </c>
@@ -8786,12 +9646,12 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -8802,7 +9662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -8825,7 +9685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>8</v>
       </c>
@@ -8848,7 +9708,7 @@
         <v>22.092325359198099</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>32</v>
       </c>
@@ -8871,7 +9731,7 @@
         <v>4.8232656449817197</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>256</v>
       </c>
@@ -8894,7 +9754,7 @@
         <v>6.2386943213578503</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2048</v>
       </c>
@@ -8917,12 +9777,12 @@
         <v>5.41536815417673</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -8936,7 +9796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>8</v>
       </c>
@@ -8951,7 +9811,7 @@
         <v>5424.432282947083</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>32</v>
       </c>
@@ -8966,7 +9826,7 @@
         <v>70575.255633700814</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>256</v>
       </c>
@@ -8981,7 +9841,7 @@
         <v>41946.515345922933</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>2048</v>
       </c>
@@ -8996,12 +9856,12 @@
         <v>37223.38461279581</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -9016,7 +9876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9024,7 +9884,7 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Redo plots and add Pec tab
</commit_message>
<xml_diff>
--- a/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
+++ b/AIMES_Experiments/Summary Files/TTC_AIMES_SWIFT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28000" windowHeight="16440" tabRatio="462" activeTab="1"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="28000" windowHeight="16440" tabRatio="462" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Timings_AIMES" sheetId="1" r:id="rId1"/>
@@ -832,66 +832,66 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="NimbusRomNo9L" charset="0"/>
-                <a:ea typeface="NimbusRomNo9L" charset="0"/>
-                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1">
+              <a:rPr lang="en-US" sz="2000" b="1" i="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="NimbusRomNo9L" charset="0"/>
-                <a:ea typeface="NimbusRomNo9L" charset="0"/>
-                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
               </a:rPr>
               <a:t>Experiment </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="NimbusRomNo9L" charset="0"/>
-                <a:ea typeface="NimbusRomNo9L" charset="0"/>
-                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
               </a:rPr>
-              <a:t>2 - </a:t>
+              <a:t>3 - </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1">
+              <a:rPr lang="en-US" sz="2000" b="1" i="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="NimbusRomNo9L" charset="0"/>
-                <a:ea typeface="NimbusRomNo9L" charset="0"/>
-                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
               </a:rPr>
-              <a:t>Tw - Swift</a:t>
+              <a:t>Tw - AIMES </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="NimbusRomNo9L" charset="0"/>
-                <a:ea typeface="NimbusRomNo9L" charset="0"/>
-                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
               </a:rPr>
-              <a:t> on Stampede and Gordon</a:t>
+              <a:t>on Stampede and Gordon</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="2000" b="1">
+            <a:endParaRPr lang="en-US" sz="2000" b="1" i="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="NimbusRomNo9L" charset="0"/>
-              <a:ea typeface="NimbusRomNo9L" charset="0"/>
-              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
@@ -924,13 +924,13 @@
             <a:buFontTx/>
             <a:buNone/>
             <a:tabLst/>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="NimbusRomNo9L" charset="0"/>
-              <a:ea typeface="NimbusRomNo9L" charset="0"/>
-              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -950,9 +950,9 @@
             <c:v>Tw</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -967,7 +967,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -980,42 +980,42 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$16:$G$19</c:f>
+                <c:f>'Plot Data'!$E$16:$E$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.0923253591981</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.82326564498172</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.23869432135785</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.41536815417673</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Plot Data'!$G$16:$G$19</c:f>
+                <c:f>'Plot Data'!$E$16:$E$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>22.0923253591981</c:v>
+                    <c:v>7.024409456368813</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.82326564498172</c:v>
+                    <c:v>19.30503716258236</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.23869432135785</c:v>
+                    <c:v>55.59854950390975</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.41536815417673</c:v>
+                    <c:v>199.5584495734066</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1057,21 +1057,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Plot Data'!$F$16:$F$19</c:f>
+              <c:f>'Plot Data'!$D$16:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>134.391339005</c:v>
+                  <c:v>128.473381339625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.683530095</c:v>
+                  <c:v>131.04659050475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.19159406</c:v>
+                  <c:v>176.592414587375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>209.6199097075</c:v>
+                  <c:v>363.74241572375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1200,7 +1200,7 @@
         <c:axId val="-2043032064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000.0"/>
+          <c:max val="4000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1393,6 +1393,1194 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+              </a:rPr>
+              <a:t>Experiment 3 - TTC on Stampede</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+                <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+              </a:rPr>
+              <a:t> and Gordon</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000" b="1" i="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TTCmeasured</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>330.5507541285718</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>160.4937990129405</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>282.4406172309012</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>734.4593988738773</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Plot Data'!$E$6:$E$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>330.5507541285718</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>160.4937990129405</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>282.4406172309012</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>734.4593988738773</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Plot Data'!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1525.89711847875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1195.15302783125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1539.4759002325</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3052.8215979325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>TTCideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Plot Data'!$H$6:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2031175488"/>
+        <c:axId val="-2031620880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2031175488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2031620880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2031620880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4000.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2031175488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Plot Data'!$G$16:$G$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>22.0923253591981</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.82326564498172</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.23869432135785</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.41536815417673</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Plot Data'!$G$16:$G$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>22.0923253591981</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.82326564498172</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.23869432135785</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.41536815417673</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Plot Data'!$A$16:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Plot Data'!$F$16:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>134.391339005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.683530095</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140.19159406</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>209.6199097075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2041535568"/>
+        <c:axId val="-2032833504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2041535568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2032833504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2032833504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4000.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2041535568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3428,7 +4616,7 @@
             <c:v>TTCmeasured</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -3563,7 +4751,7 @@
             <c:v>TTCideal</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -3752,7 +4940,7 @@
         <c:axId val="-2043514640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60000.0"/>
+          <c:max val="4000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3990,6 +5178,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5035,6 +6303,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5329,15 +7603,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>18143</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>18143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>819952</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>68062</xdr:rowOff>
+      <xdr:colOff>838095</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>86204</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5353,6 +7627,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>819952</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>68062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5396,7 +7734,7 @@
               <a:ea typeface="NimbusRomNo9L" charset="0"/>
               <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:rPr>
-            <a:t>Experiment 3 - TTC</a:t>
+            <a:t>Experiment 4 - TTC</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
@@ -5404,7 +7742,152 @@
               <a:ea typeface="NimbusRomNo9L" charset="0"/>
               <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:rPr>
-            <a:t> - AIMES on Stampede, Gordon, SuperMIC, Comet</a:t>
+            <a:t> - AIMES on Stampede, Gordon, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>SuperMIC</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:rPr>
+            <a:t>, Comet</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000" b="1">
+            <a:latin typeface="NimbusRomNo9L" charset="0"/>
+            <a:ea typeface="NimbusRomNo9L" charset="0"/>
+            <a:cs typeface="NimbusRomNo9L" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03563</cdr:x>
+      <cdr:y>0.01753</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.97695</cdr:x>
+      <cdr:y>0.09591</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="308440" y="87085"/>
+          <a:ext cx="8149655" cy="389263"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="0">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>Experiment</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:rPr>
+            <a:t> 4 - Tw</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:rPr>
+            <a:t>- AIMES on Stampede, Gordon, SuperMIC, Comet</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:latin typeface="NimbusRomNo9L" charset="0"/>
@@ -5683,7 +8166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -8814,7 +11297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5:P8"/>
     </sheetView>
   </sheetViews>
@@ -9455,7 +11938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P70:S71"/>
   <sheetViews>
-    <sheetView topLeftCell="I15" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScale="41" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
       <selection activeCell="AS77" sqref="AS77"/>
     </sheetView>
   </sheetViews>
@@ -9486,8 +11969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9810,6 +12293,10 @@
       <c r="D25">
         <v>5424.432282947083</v>
       </c>
+      <c r="G25">
+        <f>(D25/B25)*100</f>
+        <v>4275.2145852776557</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
@@ -9825,6 +12312,10 @@
       <c r="D26">
         <v>70575.255633700814</v>
       </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G28" si="1">(D26/B26)*100</f>
+        <v>41666.390154041321</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
@@ -9840,6 +12331,10 @@
       <c r="D27">
         <v>41946.515345922933</v>
       </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>29384.409285034206</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
@@ -9854,6 +12349,10 @@
       </c>
       <c r="D28">
         <v>37223.38461279581</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>1081.3052405452499</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
@@ -9880,8 +12379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>